<commit_message>
added a bunch of experimental metadata (without SWATE)
</commit_message>
<xml_diff>
--- a/assays/Talinum_RNASeq_minimal/assay.isa.xlsx
+++ b/assays/Talinum_RNASeq_minimal/assay.isa.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10711"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10808"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/sciebo/CEPLAS_DM/CEPLAS_ARCs/ARC0005/assays/Talinum_RNASeq_minimal/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/dominikbrilhaus/Hackathon_ARCexample_rnaseq/assays/Talinum_RNASeq_minimal/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB3D1F26-7CB7-E541-9417-AC2C0E724B2A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91EDF5AE-B8A3-294B-B9B3-4B2263017720}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2000" yWindow="-19580" windowWidth="35680" windowHeight="17500" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1SPL01_plants" sheetId="1" r:id="rId1"/>
@@ -19,12 +19,12 @@
     <sheet name="4COM01_RNASeq" sheetId="5" r:id="rId4"/>
     <sheet name="Investigation" sheetId="2" r:id="rId5"/>
   </sheets>
-  <calcPr calcId="0"/>
+  <calcPr calcId="191029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="360" uniqueCount="276">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="537" uniqueCount="324">
   <si>
     <t>ASSAY METADATA</t>
   </si>
@@ -701,9 +701,6 @@
     <t>Term Accession Number [Library strategy] (#h; #tNFDI4PSO:0000035)</t>
   </si>
   <si>
-    <t>RNA-Seq Assay</t>
-  </si>
-  <si>
     <t>Parameter [Processed data file checksum]</t>
   </si>
   <si>
@@ -852,6 +849,153 @@
   </si>
   <si>
     <t>2 days rewatered</t>
+  </si>
+  <si>
+    <t>DB_097</t>
+  </si>
+  <si>
+    <t>DB_099</t>
+  </si>
+  <si>
+    <t>DB_103</t>
+  </si>
+  <si>
+    <t>DB_161</t>
+  </si>
+  <si>
+    <t>DB_163</t>
+  </si>
+  <si>
+    <t>DB_165</t>
+  </si>
+  <si>
+    <t>28 days after germination</t>
+  </si>
+  <si>
+    <t>growth chamber study</t>
+  </si>
+  <si>
+    <t>PECO</t>
+  </si>
+  <si>
+    <t>http://purl.obolibrary.org/obo/PECO_0007269</t>
+  </si>
+  <si>
+    <t>Parameter [growth chamber company]</t>
+  </si>
+  <si>
+    <t>Environmental Growth Chambers, Ohio</t>
+  </si>
+  <si>
+    <t>Miracle-Gro Potting Mix</t>
+  </si>
+  <si>
+    <t>Term Source REF [growth chamber company] (#h)</t>
+  </si>
+  <si>
+    <t>Term Accession Number [growth chamber company] (#h)</t>
+  </si>
+  <si>
+    <t>Parameter [Flower pot]</t>
+  </si>
+  <si>
+    <t>Term Source REF [Flower pot] (#h)</t>
+  </si>
+  <si>
+    <t>Term Accession Number [Flower pot] (#h)</t>
+  </si>
+  <si>
+    <t>Stuewe and Sons "Short-One" treepots, 1.6 L</t>
+  </si>
+  <si>
+    <t>12 hr light / 12 hr dark</t>
+  </si>
+  <si>
+    <t>Shock-freeze in liquid nitrogen</t>
+  </si>
+  <si>
+    <t>6 Zeitgeber time</t>
+  </si>
+  <si>
+    <t>7 Zeitgeber time</t>
+  </si>
+  <si>
+    <t>8 Zeitgeber time</t>
+  </si>
+  <si>
+    <t>AGTCAA</t>
+  </si>
+  <si>
+    <t>GTCCGC</t>
+  </si>
+  <si>
+    <t>GTGAAA</t>
+  </si>
+  <si>
+    <t>CAGATC</t>
+  </si>
+  <si>
+    <t>CTTGTA</t>
+  </si>
+  <si>
+    <t>mRNA</t>
+  </si>
+  <si>
+    <t>Roboklon EURx GeneMATRIX Universal RNA Purification version 2.3 September 2011</t>
+  </si>
+  <si>
+    <t>RIN 7.6 (Agilent Bioanalyzer 2100 expert_Plant RNA Nano)</t>
+  </si>
+  <si>
+    <t>RIN 7.7 (Agilent Bioanalyzer 2100 expert_Plant RNA Nano)</t>
+  </si>
+  <si>
+    <t>RIN 6.5 (Agilent Bioanalyzer 2100 expert_Plant RNA Nano)</t>
+  </si>
+  <si>
+    <t>RIN 7.8 (Agilent Bioanalyzer 2100 expert_Plant RNA Nano)</t>
+  </si>
+  <si>
+    <t>Roboklon commercial buffers</t>
+  </si>
+  <si>
+    <t>*.fastq.gz</t>
+  </si>
+  <si>
+    <t>Forward</t>
+  </si>
+  <si>
+    <t>Illumina TruSeq RNA Sample Prep Kit</t>
+  </si>
+  <si>
+    <t>version 2</t>
+  </si>
+  <si>
+    <t>DNase (New England Biolabs)</t>
+  </si>
+  <si>
+    <t>single</t>
+  </si>
+  <si>
+    <t>RNA-Seq</t>
+  </si>
+  <si>
+    <t>cDNA method</t>
+  </si>
+  <si>
+    <t>Illumina Cassava</t>
+  </si>
+  <si>
+    <t>v1.8.2</t>
+  </si>
+  <si>
+    <t>Illumina HiSeq 2000 Rapid Run</t>
+  </si>
+  <si>
+    <t>BLAT</t>
+  </si>
+  <si>
+    <t>Arabidopsis TAIR10 CDS</t>
   </si>
 </sst>
 </file>
@@ -1016,7 +1160,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1202,8 +1346,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor theme="9" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="13">
+  <borders count="14">
     <border>
       <left/>
       <right/>
@@ -1347,6 +1497,17 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="9" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="42">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -1392,7 +1553,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="33" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1410,6 +1571,11 @@
     <xf numFmtId="0" fontId="18" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="18" fillId="33" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="34" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="13" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="42">
     <cellStyle name="20% - Accent1" xfId="19" builtinId="30" customBuiltin="1"/>
@@ -1455,18 +1621,64 @@
     <cellStyle name="Total" xfId="17" builtinId="25" customBuiltin="1"/>
     <cellStyle name="Warning Text" xfId="14" builtinId="11" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="73">
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
+  <dxfs count="75">
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike val="0"/>
+        <condense val="0"/>
+        <extend val="0"/>
+        <outline val="0"/>
+        <shadow val="0"/>
+        <u val="none"/>
+        <vertAlign val="baseline"/>
+        <sz val="12"/>
+        <color theme="1"/>
+        <name val="Calibri"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </font>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </top>
+        <bottom style="thin">
+          <color theme="9" tint="0.39997558519241921"/>
+        </bottom>
+        <vertical/>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -1547,9 +1759,6 @@
       <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="168" formatCode="0.00\ &quot;microliter&quot;"/>
     </dxf>
     <dxf>
@@ -1611,15 +1820,6 @@
     </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.00\ &quot;microeinstein per square meter per second&quot;"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
     </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
@@ -1689,134 +1889,140 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42878A1A-AB6B-BD4C-9AA4-881DB03B9D90}" name="annotationTable" displayName="annotationTable" ref="A2:DX8" totalsRowShown="0">
-  <autoFilter ref="A2:DX8" xr:uid="{42878A1A-AB6B-BD4C-9AA4-881DB03B9D90}"/>
-  <tableColumns count="128">
-    <tableColumn id="1" xr3:uid="{1AC7FA6D-F4A4-9443-B0D0-921B6A5822B2}" name="Source Name"/>
-    <tableColumn id="126" xr3:uid="{34D5E4DA-6008-0D4F-92B4-60D9A4BA1820}" name="Characteristics [Sample type]" dataDxfId="72"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{42878A1A-AB6B-BD4C-9AA4-881DB03B9D90}" name="annotationTable" displayName="annotationTable" ref="A2:ED8" totalsRowShown="0">
+  <autoFilter ref="A2:ED8" xr:uid="{42878A1A-AB6B-BD4C-9AA4-881DB03B9D90}"/>
+  <tableColumns count="134">
+    <tableColumn id="1" xr3:uid="{1AC7FA6D-F4A4-9443-B0D0-921B6A5822B2}" name="Source Name" dataDxfId="9"/>
+    <tableColumn id="126" xr3:uid="{34D5E4DA-6008-0D4F-92B4-60D9A4BA1820}" name="Characteristics [Sample type]" dataDxfId="74"/>
     <tableColumn id="127" xr3:uid="{FE30A59B-FD0E-044A-9F22-017E078D3F6A}" name="Term Source REF [Sample type] (#h; #tNFDI4PSO:0000064)"/>
     <tableColumn id="128" xr3:uid="{86E8E2C5-0F8A-6544-994A-3DB5F7E6513B}" name="Term Accession Number [Sample type] (#h; #tNFDI4PSO:0000064)"/>
-    <tableColumn id="123" xr3:uid="{656B6EB2-9C19-604F-81FC-7EA58AB56B3C}" name="Characteristics [Biological replicate]" dataDxfId="71"/>
+    <tableColumn id="123" xr3:uid="{656B6EB2-9C19-604F-81FC-7EA58AB56B3C}" name="Characteristics [Biological replicate]" dataDxfId="73"/>
     <tableColumn id="124" xr3:uid="{88B4C827-D22C-CC41-A939-84DE2BE86C05}" name="Term Source REF [Biological replicate] (#h; #tNFDI4PSO:0000042)"/>
     <tableColumn id="125" xr3:uid="{EDD41B94-EFF8-5840-81D9-D6591F7EA0A9}" name="Term Accession Number [Biological replicate] (#h; #tNFDI4PSO:0000042)"/>
-    <tableColumn id="120" xr3:uid="{107DF550-568B-1640-9AA1-0BD5A818E6BB}" name="Characteristics [Organism]" dataDxfId="70"/>
+    <tableColumn id="120" xr3:uid="{107DF550-568B-1640-9AA1-0BD5A818E6BB}" name="Characteristics [Organism]" dataDxfId="72"/>
     <tableColumn id="121" xr3:uid="{F555C0D2-64F4-014B-8108-E98F3E5DE02E}" name="Term Source REF [Organism] (#h; #tNFDI4PSO:0000030)"/>
     <tableColumn id="122" xr3:uid="{3630B389-4AB7-DC44-A667-56461737F01A}" name="Term Accession Number [Organism] (#h; #tNFDI4PSO:0000030)"/>
-    <tableColumn id="117" xr3:uid="{EA02B49F-B0B0-1543-934D-AEAC8A05E617}" name="Characteristics [Isolate]" dataDxfId="69"/>
+    <tableColumn id="117" xr3:uid="{EA02B49F-B0B0-1543-934D-AEAC8A05E617}" name="Characteristics [Isolate]" dataDxfId="71"/>
     <tableColumn id="118" xr3:uid="{D90196FB-CDFE-D747-9BF9-9746844877BE}" name="Term Source REF [Isolate] (#h; #tNFDI4PSO:0000065)"/>
     <tableColumn id="119" xr3:uid="{F8E90BC8-01DE-1B42-B494-A07B7EA50639}" name="Term Accession Number [Isolate] (#h; #tNFDI4PSO:0000065)"/>
-    <tableColumn id="114" xr3:uid="{EB28AFC6-1732-F94D-A368-2C0B70E2D3AF}" name="Characteristics [Cultivar]" dataDxfId="68"/>
+    <tableColumn id="114" xr3:uid="{EB28AFC6-1732-F94D-A368-2C0B70E2D3AF}" name="Characteristics [Cultivar]" dataDxfId="70"/>
     <tableColumn id="115" xr3:uid="{DBED37C8-A247-7141-912F-98A0EDDDA227}" name="Term Source REF [Cultivar] (#h; #tNFDI4PSO:0000066)"/>
     <tableColumn id="116" xr3:uid="{0E2D305B-59CD-BA49-90D4-63A0F3A94456}" name="Term Accession Number [Cultivar] (#h; #tNFDI4PSO:0000066)"/>
-    <tableColumn id="111" xr3:uid="{2B6EC663-4B60-8C40-B399-3A6D22E596F2}" name="Characteristics [Ecotype]" dataDxfId="67"/>
+    <tableColumn id="111" xr3:uid="{2B6EC663-4B60-8C40-B399-3A6D22E596F2}" name="Characteristics [Ecotype]" dataDxfId="69"/>
     <tableColumn id="112" xr3:uid="{31D2F19E-A389-CF45-98FD-1732C3A7A250}" name="Term Source REF [Ecotype] (#h; #tNFDI4PSO:0000067)"/>
     <tableColumn id="113" xr3:uid="{0A125659-0A85-8447-A031-89C1D0BBC321}" name="Term Accession Number [Ecotype] (#h; #tNFDI4PSO:0000067)"/>
-    <tableColumn id="108" xr3:uid="{DDF34AC5-5889-6143-94E0-4C83CE461189}" name="Characteristics [Genotype]" dataDxfId="66"/>
+    <tableColumn id="108" xr3:uid="{DDF34AC5-5889-6143-94E0-4C83CE461189}" name="Characteristics [Genotype]" dataDxfId="68"/>
     <tableColumn id="109" xr3:uid="{86B35B7D-6DDA-484B-87CF-B258A23011C7}" name="Term Source REF [Genotype] (#h; #tNFDI4PSO:0000031)"/>
     <tableColumn id="110" xr3:uid="{3DC28CE4-6A7A-DF46-976D-6A0FB3283A94}" name="Term Accession Number [Genotype] (#h; #tNFDI4PSO:0000031)"/>
-    <tableColumn id="105" xr3:uid="{5FE48726-A26D-C84E-8618-10D1BC1B8D21}" name="Characteristics [population]" dataDxfId="65"/>
+    <tableColumn id="105" xr3:uid="{5FE48726-A26D-C84E-8618-10D1BC1B8D21}" name="Characteristics [population]" dataDxfId="67"/>
     <tableColumn id="106" xr3:uid="{CD83B2FB-4899-EA46-A6D8-4C8F237E894E}" name="Term Source REF [population] (#h; #tOBI:0000181)"/>
     <tableColumn id="107" xr3:uid="{184D1E0B-57BD-8E42-A340-48D860433969}" name="Term Accession Number [population] (#h; #tOBI:0000181)"/>
-    <tableColumn id="102" xr3:uid="{66CFA3B9-B531-6641-9698-BB5EA70CCF50}" name="Characteristics [Organism part]" dataDxfId="64"/>
+    <tableColumn id="102" xr3:uid="{66CFA3B9-B531-6641-9698-BB5EA70CCF50}" name="Characteristics [Organism part]" dataDxfId="66"/>
     <tableColumn id="103" xr3:uid="{F6E1C8DC-8734-CD48-BB18-CD710C787A54}" name="Term Source REF [Organism part] (#h; #tNFDI4PSO:0000032)"/>
     <tableColumn id="104" xr3:uid="{D53E1174-E962-5249-9F35-48E62817A44E}" name="Term Accession Number [Organism part] (#h; #tNFDI4PSO:0000032)"/>
-    <tableColumn id="99" xr3:uid="{6455468B-6E31-6F41-AFBC-EECB92A8CF8E}" name="Characteristics [Cell line]" dataDxfId="63"/>
+    <tableColumn id="99" xr3:uid="{6455468B-6E31-6F41-AFBC-EECB92A8CF8E}" name="Characteristics [Cell line]" dataDxfId="65"/>
     <tableColumn id="100" xr3:uid="{C53B236E-F015-6849-BE9B-AFED976B811A}" name="Term Source REF [Cell line] (#h; #tNFDI4PSO:0000068)"/>
     <tableColumn id="101" xr3:uid="{54D639E1-ED3C-D244-AC34-EEC7039B9112}" name="Term Accession Number [Cell line] (#h; #tNFDI4PSO:0000068)"/>
-    <tableColumn id="96" xr3:uid="{E1FC3826-471C-B14B-BD18-0DFE7542F06F}" name="Characteristics [Cell type]" dataDxfId="62"/>
+    <tableColumn id="96" xr3:uid="{E1FC3826-471C-B14B-BD18-0DFE7542F06F}" name="Characteristics [Cell type]" dataDxfId="64"/>
     <tableColumn id="97" xr3:uid="{5782AF59-601F-B14D-8839-4005B524452E}" name="Term Source REF [Cell type] (#h; #tNFDI4PSO:0000069)"/>
     <tableColumn id="98" xr3:uid="{9BD9EDD0-280E-AA46-ABDC-F1F9E7C5793C}" name="Term Accession Number [Cell type] (#h; #tNFDI4PSO:0000069)"/>
-    <tableColumn id="93" xr3:uid="{78B66C9B-6BEF-C644-BA73-87EDFBE2317A}" name="Characteristics [age]" dataDxfId="61"/>
+    <tableColumn id="93" xr3:uid="{78B66C9B-6BEF-C644-BA73-87EDFBE2317A}" name="Characteristics [age]" dataDxfId="7"/>
     <tableColumn id="94" xr3:uid="{04749508-9B5B-9343-888A-2C42ED3C5076}" name="Term Source REF [age] (#h; #tNFDI4PSO:0000033)"/>
     <tableColumn id="95" xr3:uid="{09EBB8A0-FCFB-DB41-BAE2-18754BBF4367}" name="Term Accession Number [age] (#h; #tNFDI4PSO:0000033)"/>
-    <tableColumn id="90" xr3:uid="{0154ABFB-076C-8F49-8911-F9670D6A9D5D}" name="Characteristics [Developmental Stage]" dataDxfId="60"/>
+    <tableColumn id="90" xr3:uid="{0154ABFB-076C-8F49-8911-F9670D6A9D5D}" name="Characteristics [Developmental Stage]" dataDxfId="63"/>
     <tableColumn id="91" xr3:uid="{6D879866-AF2B-4741-8248-0DE47FF7280E}" name="Term Source REF [Developmental Stage] (#h; #tNFDI4PSO:0000070)"/>
     <tableColumn id="92" xr3:uid="{9EE8AE2E-07C2-764A-A01D-B8D25093B2F6}" name="Term Accession Number [Developmental Stage] (#h; #tNFDI4PSO:0000070)"/>
-    <tableColumn id="87" xr3:uid="{2BDA0C5B-8DA4-4A46-AF94-C1359747DFC9}" name="Characteristics [Plant disease]" dataDxfId="59"/>
+    <tableColumn id="87" xr3:uid="{2BDA0C5B-8DA4-4A46-AF94-C1359747DFC9}" name="Characteristics [Plant disease]" dataDxfId="62"/>
     <tableColumn id="88" xr3:uid="{930E90DE-0FFB-1B49-9B8D-1604FB5E5DB9}" name="Term Source REF [Plant disease] (#h; #tNFDI4PSO:0000071)"/>
     <tableColumn id="89" xr3:uid="{CA62CE2F-B67F-BD4D-987C-C6F16BC43D11}" name="Term Accession Number [Plant disease] (#h; #tNFDI4PSO:0000071)"/>
-    <tableColumn id="84" xr3:uid="{B23091A0-4954-3143-B091-AD1B22891673}" name="Characteristics [Plant disease stage]" dataDxfId="58"/>
+    <tableColumn id="84" xr3:uid="{B23091A0-4954-3143-B091-AD1B22891673}" name="Characteristics [Plant disease stage]" dataDxfId="61"/>
     <tableColumn id="85" xr3:uid="{D35074E2-CA91-1B4B-B030-07ECB6B9074B}" name="Term Source REF [Plant disease stage] (#h; #tNFDI4PSO:0000072)"/>
     <tableColumn id="86" xr3:uid="{26AA6338-7B29-7C4B-91A5-D1EA38D921B7}" name="Term Accession Number [Plant disease stage] (#h; #tNFDI4PSO:0000072)"/>
-    <tableColumn id="81" xr3:uid="{0867E5AB-8482-FF4D-8B7C-CAA2E822EA3E}" name="Characteristics [Phenotype]" dataDxfId="57"/>
+    <tableColumn id="81" xr3:uid="{0867E5AB-8482-FF4D-8B7C-CAA2E822EA3E}" name="Characteristics [Phenotype]" dataDxfId="60"/>
     <tableColumn id="82" xr3:uid="{226E6233-564E-A74E-94F5-EA84CA520B99}" name="Term Source REF [Phenotype] (#h; #tNFDI4PSO:0000073)"/>
     <tableColumn id="83" xr3:uid="{71A34F30-BAD0-DB4C-962D-42800C2A0880}" name="Term Accession Number [Phenotype] (#h; #tNFDI4PSO:0000073)"/>
-    <tableColumn id="78" xr3:uid="{A51828EB-D510-964C-894D-5368BFA61056}" name="Characteristics [whole plant size]" dataDxfId="56"/>
+    <tableColumn id="78" xr3:uid="{A51828EB-D510-964C-894D-5368BFA61056}" name="Characteristics [whole plant size]" dataDxfId="59"/>
     <tableColumn id="79" xr3:uid="{CABEA748-7180-3948-88A4-B1D7E0C4953C}" name="Term Source REF [whole plant size] (#h; #tTO:1000012)"/>
     <tableColumn id="80" xr3:uid="{EE7C023B-5B51-2046-9F8E-D7137F516328}" name="Term Accession Number [whole plant size] (#h; #tTO:1000012)"/>
-    <tableColumn id="75" xr3:uid="{86286C9D-15DE-C241-AED2-02FC433166B9}" name="Characteristics [study type]" dataDxfId="55"/>
+    <tableColumn id="75" xr3:uid="{86286C9D-15DE-C241-AED2-02FC433166B9}" name="Characteristics [study type]" dataDxfId="58"/>
     <tableColumn id="76" xr3:uid="{4F11CDED-2386-D740-ABD1-DED5E5AFA9D2}" name="Term Source REF [study type] (#h; #tPECO:0007231)"/>
     <tableColumn id="77" xr3:uid="{AA165248-200B-464E-B9AC-8DF6D66A9307}" name="Term Accession Number [study type] (#h; #tPECO:0007231)"/>
-    <tableColumn id="72" xr3:uid="{04EA63C7-AF88-F54E-8565-8DAE1BBCC6DD}" name="Characteristics [plant growth medium exposure]" dataDxfId="54"/>
+    <tableColumn id="129" xr3:uid="{C399A8D1-E8A5-3649-964F-AE2FB7774EB3}" name="Parameter [growth chamber company]" dataDxfId="6"/>
+    <tableColumn id="131" xr3:uid="{E74397EF-7DE4-2B43-97B4-02956DB76284}" name="Term Source REF [growth chamber company] (#h)" dataDxfId="3"/>
+    <tableColumn id="130" xr3:uid="{EC06A69F-E75F-B040-BEC4-68FAFD158B9C}" name="Term Accession Number [growth chamber company] (#h)" dataDxfId="4"/>
+    <tableColumn id="72" xr3:uid="{04EA63C7-AF88-F54E-8565-8DAE1BBCC6DD}" name="Characteristics [plant growth medium exposure]" dataDxfId="5"/>
     <tableColumn id="73" xr3:uid="{CD4D5A49-A0F1-B54A-91AA-D33A38B60508}" name="Term Source REF [plant growth medium exposure] (#h; #tPECO:0007147)"/>
     <tableColumn id="74" xr3:uid="{9E63E743-F2ED-DA41-B695-5F814E4F130D}" name="Term Accession Number [plant growth medium exposure] (#h; #tPECO:0007147)"/>
-    <tableColumn id="69" xr3:uid="{26C13274-5C42-AD46-886F-688C25E249B9}" name="Characteristics [growth plot design]" dataDxfId="53"/>
+    <tableColumn id="134" xr3:uid="{044B8EE6-C065-4743-9684-2B0B1B26A535}" name="Parameter [Flower pot]"/>
+    <tableColumn id="133" xr3:uid="{002BB076-520E-C946-8435-24B46AFC612F}" name="Term Source REF [Flower pot] (#h)"/>
+    <tableColumn id="132" xr3:uid="{3780BA6B-6E59-1342-A3D3-563AF8DF74C5}" name="Term Accession Number [Flower pot] (#h)"/>
+    <tableColumn id="69" xr3:uid="{26C13274-5C42-AD46-886F-688C25E249B9}" name="Characteristics [growth plot design]" dataDxfId="57"/>
     <tableColumn id="70" xr3:uid="{EB2844CE-DBFA-2548-B488-7A0BE10115DA}" name="Term Source REF [growth plot design] (#h; #tNFDI4PSO:0000001)"/>
     <tableColumn id="71" xr3:uid="{0066F752-AFE5-B44F-9E88-63E759515140}" name="Term Accession Number [growth plot design] (#h; #tNFDI4PSO:0000001)"/>
-    <tableColumn id="66" xr3:uid="{8F77373D-F219-6F45-96BD-A2514A6DE070}" name="Characteristics [Growth day length]" dataDxfId="52"/>
+    <tableColumn id="66" xr3:uid="{8F77373D-F219-6F45-96BD-A2514A6DE070}" name="Characteristics [Growth day length]" dataDxfId="2"/>
     <tableColumn id="67" xr3:uid="{DC58F327-13D0-B64B-A96A-3EA3A52B75EA}" name="Term Source REF [Growth day length] (#h; #tNFDI4PSO:0000041)"/>
     <tableColumn id="68" xr3:uid="{F12CE813-E100-954F-A7F5-33D31F0FCDA1}" name="Term Accession Number [Growth day length] (#h; #tNFDI4PSO:0000041)"/>
-    <tableColumn id="60" xr3:uid="{C97F32D4-721B-A44D-AF40-6DD5C01BF304}" name="Characteristics [light intensity exposure]" dataDxfId="51"/>
+    <tableColumn id="60" xr3:uid="{C97F32D4-721B-A44D-AF40-6DD5C01BF304}" name="Characteristics [light intensity exposure]" dataDxfId="56"/>
     <tableColumn id="61" xr3:uid="{A2EA9D83-B7DE-EA44-9B63-9FD99E1AF6E2}" name="Term Source REF [light intensity exposure] (#h; #tPECO:0007224)"/>
     <tableColumn id="62" xr3:uid="{3ABEEA3E-45B8-5640-A86B-1E64B4382A01}" name="Term Accession Number [light intensity exposure] (#h; #tPECO:0007224)"/>
     <tableColumn id="63" xr3:uid="{DA5CA42C-2FD9-7745-9BE6-3CB08A75B3D5}" name="Unit [microeinstein per square meter per second] (#h; #tUO:0000160; #u)"/>
     <tableColumn id="64" xr3:uid="{19C7FF60-E4D9-4945-BABF-9A97CE261595}" name="Term Source REF [microeinstein per square meter per second] (#h; #tUO:0000160; #u)"/>
     <tableColumn id="65" xr3:uid="{F1EC31D1-1E0E-D943-85A5-72EC851440F7}" name="Term Accession Number [microeinstein per square meter per second] (#h; #tUO:0000160; #u)"/>
-    <tableColumn id="54" xr3:uid="{8C36C182-222C-0B4A-A53C-46FD311C6979}" name="Characteristics [Humidity Day]" dataDxfId="50"/>
+    <tableColumn id="54" xr3:uid="{8C36C182-222C-0B4A-A53C-46FD311C6979}" name="Characteristics [Humidity Day]" dataDxfId="55"/>
     <tableColumn id="55" xr3:uid="{175F5D5A-8C38-7B46-86C7-C846E5CB43BF}" name="Term Source REF [Humidity Day] (#h; #tNFDI4PSO:0000005)"/>
     <tableColumn id="56" xr3:uid="{E57934AD-3A87-464D-9ADE-301562F43380}" name="Term Accession Number [Humidity Day] (#h; #tNFDI4PSO:0000005)"/>
     <tableColumn id="57" xr3:uid="{F9D9E7B2-A5C7-734C-99A4-BC82650C2638}" name="Unit [percent] (#2; #h; #tUO:0000187; #u)"/>
     <tableColumn id="58" xr3:uid="{7AE058A9-3D06-0740-AF61-652C084AF134}" name="Term Source REF [percent] (#2; #h; #tUO:0000187; #u)"/>
     <tableColumn id="59" xr3:uid="{AD2C96D4-9F19-A648-A07A-708D67DCFD2C}" name="Term Accession Number [percent] (#2; #h; #tUO:0000187; #u)"/>
-    <tableColumn id="48" xr3:uid="{7036BC3C-5B89-7846-9099-315C6AB9E703}" name="Characteristics [Humidity Night]" dataDxfId="49"/>
+    <tableColumn id="48" xr3:uid="{7036BC3C-5B89-7846-9099-315C6AB9E703}" name="Characteristics [Humidity Night]" dataDxfId="54"/>
     <tableColumn id="49" xr3:uid="{1A7F7497-5A36-1047-8727-2EEF86674FA3}" name="Term Source REF [Humidity Night] (#h; #tNFDI4PSO:0000006)"/>
     <tableColumn id="50" xr3:uid="{B0DC73EA-8814-B642-92C9-5F720E297119}" name="Term Accession Number [Humidity Night] (#h; #tNFDI4PSO:0000006)"/>
     <tableColumn id="51" xr3:uid="{46616EBB-F37B-5B4E-8BED-472AB9C239C1}" name="Unit [percent] (#h; #tUO:0000187; #u)"/>
     <tableColumn id="52" xr3:uid="{34764718-C809-7040-BAF7-66D5AF999C04}" name="Term Source REF [percent] (#h; #tUO:0000187; #u)"/>
     <tableColumn id="53" xr3:uid="{A05BC216-DB33-7E47-8C61-824BBEA6B60D}" name="Term Accession Number [percent] (#h; #tUO:0000187; #u)"/>
-    <tableColumn id="42" xr3:uid="{83102DA5-6D6D-6E47-842A-FDF81BBC78FE}" name="Characteristics [Temperature Day]" dataDxfId="48"/>
+    <tableColumn id="42" xr3:uid="{83102DA5-6D6D-6E47-842A-FDF81BBC78FE}" name="Characteristics [Temperature Day]" dataDxfId="53"/>
     <tableColumn id="43" xr3:uid="{9031C13E-B5A2-8146-BD88-C2BC147FEDE6}" name="Term Source REF [Temperature Day] (#h; #tNFDI4PSO:0000007)"/>
     <tableColumn id="44" xr3:uid="{741EB9FA-D628-B549-8343-BE6E0AA13744}" name="Term Accession Number [Temperature Day] (#h; #tNFDI4PSO:0000007)"/>
     <tableColumn id="45" xr3:uid="{D2372BB1-6F20-9A44-87F8-7D6CC0120E8F}" name="Unit [degree Celsius] (#2; #h; #tUO:0000027; #u)"/>
     <tableColumn id="46" xr3:uid="{2C42B93C-AA73-6949-81DC-4E1E959E7DB0}" name="Term Source REF [degree Celsius] (#2; #h; #tUO:0000027; #u)"/>
     <tableColumn id="47" xr3:uid="{4B7D0427-FC86-6D44-B186-9235FE27CBE8}" name="Term Accession Number [degree Celsius] (#2; #h; #tUO:0000027; #u)"/>
-    <tableColumn id="36" xr3:uid="{2AFCA422-9D7C-8743-AA8C-93A4C122D886}" name="Characteristics [Temperature Night]" dataDxfId="47"/>
+    <tableColumn id="36" xr3:uid="{2AFCA422-9D7C-8743-AA8C-93A4C122D886}" name="Characteristics [Temperature Night]" dataDxfId="52"/>
     <tableColumn id="37" xr3:uid="{DD90420D-6650-8140-9D90-9CE8D9399E72}" name="Term Source REF [Temperature Night] (#h; #tNFDI4PSO:0000008)"/>
     <tableColumn id="38" xr3:uid="{870F321E-F154-B340-A408-834F17B5D7E7}" name="Term Accession Number [Temperature Night] (#h; #tNFDI4PSO:0000008)"/>
     <tableColumn id="39" xr3:uid="{3361F32D-097A-794D-9663-0813525728EF}" name="Unit [degree Celsius] (#h; #tUO:0000027; #u)"/>
     <tableColumn id="40" xr3:uid="{92BC8292-8611-D948-8A25-72820BF0E708}" name="Term Source REF [degree Celsius] (#h; #tUO:0000027; #u)"/>
     <tableColumn id="41" xr3:uid="{200E566C-E890-B843-B4C7-6954BCCC6930}" name="Term Accession Number [degree Celsius] (#h; #tUO:0000027; #u)"/>
-    <tableColumn id="33" xr3:uid="{B326ED90-F0FA-5548-809C-8D4168F77B91}" name="Characteristics [watering exposure]" dataDxfId="46"/>
+    <tableColumn id="33" xr3:uid="{B326ED90-F0FA-5548-809C-8D4168F77B91}" name="Characteristics [watering exposure]" dataDxfId="51"/>
     <tableColumn id="34" xr3:uid="{7AD95EDD-18C4-A140-91D9-3D184F4A24C9}" name="Term Source REF [watering exposure] (#h; #tPECO:0007383)"/>
     <tableColumn id="35" xr3:uid="{75DAE13B-A28C-4B4C-A75C-350F50030C86}" name="Term Accession Number [watering exposure] (#h; #tPECO:0007383)"/>
-    <tableColumn id="30" xr3:uid="{A23F0E1E-2786-304E-A46C-4154A9006918}" name="Characteristics [plant nutrient exposure]" dataDxfId="45"/>
+    <tableColumn id="30" xr3:uid="{A23F0E1E-2786-304E-A46C-4154A9006918}" name="Characteristics [plant nutrient exposure]" dataDxfId="50"/>
     <tableColumn id="31" xr3:uid="{31101F85-8A4F-254A-AB05-97B62543D86D}" name="Term Source REF [plant nutrient exposure] (#h; #tPECO:0007241)"/>
     <tableColumn id="32" xr3:uid="{BFC91796-0423-3E47-A440-46412F9EB8CD}" name="Term Accession Number [plant nutrient exposure] (#h; #tPECO:0007241)"/>
-    <tableColumn id="27" xr3:uid="{D0A9A0C3-7AEE-EE4A-9906-3EABA49B033E}" name="Characteristics [abiotic plant exposure]" dataDxfId="44"/>
+    <tableColumn id="27" xr3:uid="{D0A9A0C3-7AEE-EE4A-9906-3EABA49B033E}" name="Characteristics [abiotic plant exposure]" dataDxfId="49"/>
     <tableColumn id="28" xr3:uid="{CACFFC75-EE24-7A4F-AB5E-27FAD7798275}" name="Term Source REF [abiotic plant exposure] (#h; #tPECO:0007191)"/>
     <tableColumn id="29" xr3:uid="{AC071C3E-EEC1-6249-A69A-486CCEDE6FCC}" name="Term Accession Number [abiotic plant exposure] (#h; #tPECO:0007191)"/>
-    <tableColumn id="24" xr3:uid="{5A5877BF-6940-C848-A817-70B1234B0CF6}" name="Characteristics [biotic plant exposure]" dataDxfId="43"/>
+    <tableColumn id="24" xr3:uid="{5A5877BF-6940-C848-A817-70B1234B0CF6}" name="Characteristics [biotic plant exposure]" dataDxfId="48"/>
     <tableColumn id="25" xr3:uid="{DFCFC6F8-A8EA-2340-A466-BBB92A36A9C2}" name="Term Source REF [biotic plant exposure] (#h; #tPECO:0007357)"/>
     <tableColumn id="26" xr3:uid="{4D9938A4-4BC7-8045-8B11-F71F538FAE82}" name="Term Accession Number [biotic plant exposure] (#h; #tPECO:0007357)"/>
-    <tableColumn id="21" xr3:uid="{4B4D4ADD-1644-004A-B170-ABB3E5133349}" name="Characteristics [Geographic Area]" dataDxfId="42"/>
+    <tableColumn id="21" xr3:uid="{4B4D4ADD-1644-004A-B170-ABB3E5133349}" name="Characteristics [Geographic Area]" dataDxfId="47"/>
     <tableColumn id="22" xr3:uid="{B94A8E18-14D5-2F46-A881-77C151B4CCB8}" name="Term Source REF [Geographic Area] (#h; #tNFDI4PSO:0000074)"/>
     <tableColumn id="23" xr3:uid="{6CDA0DA4-5474-524E-AAF1-CA4D6F999358}" name="Term Accession Number [Geographic Area] (#h; #tNFDI4PSO:0000074)"/>
-    <tableColumn id="18" xr3:uid="{843EBA99-BE36-5346-8066-96DCF0C497E5}" name="Characteristics [Sample Collection Date]" dataDxfId="41"/>
+    <tableColumn id="18" xr3:uid="{843EBA99-BE36-5346-8066-96DCF0C497E5}" name="Characteristics [Sample Collection Date]" dataDxfId="46"/>
     <tableColumn id="19" xr3:uid="{B1AF23FD-928D-B346-99FA-83BAC010D169}" name="Term Source REF [Sample Collection Date] (#h; #tNFDI4PSO:0000075)"/>
     <tableColumn id="20" xr3:uid="{9468896C-16F7-6B4A-82FE-DFB83922A462}" name="Term Accession Number [Sample Collection Date] (#h; #tNFDI4PSO:0000075)"/>
-    <tableColumn id="15" xr3:uid="{72AC1C27-1CF6-4243-8ADD-FAEF6C58EA32}" name="Characteristics [Sample Collected By]" dataDxfId="40"/>
+    <tableColumn id="15" xr3:uid="{72AC1C27-1CF6-4243-8ADD-FAEF6C58EA32}" name="Characteristics [Sample Collected By]" dataDxfId="45"/>
     <tableColumn id="16" xr3:uid="{36928446-E96A-B146-AA9A-A202AC1BD4E6}" name="Term Source REF [Sample Collected By] (#h; #tNFDI4PSO:0000076)"/>
     <tableColumn id="17" xr3:uid="{E516F9F7-E843-DC42-810B-9A2598F8C2A4}" name="Term Accession Number [Sample Collected By] (#h; #tNFDI4PSO:0000076)"/>
-    <tableColumn id="12" xr3:uid="{8B6BC8A5-9354-8143-A76F-97DE4D3C76D2}" name="Characteristics [Time point]" dataDxfId="39"/>
+    <tableColumn id="12" xr3:uid="{8B6BC8A5-9354-8143-A76F-97DE4D3C76D2}" name="Characteristics [Time point]" dataDxfId="44"/>
     <tableColumn id="13" xr3:uid="{75E80241-B3A5-4348-A9DF-0509262ECEF2}" name="Term Source REF [Time point] (#h; #tNFDI4PSO:0000034)"/>
     <tableColumn id="14" xr3:uid="{1996F0D4-E712-8243-A26B-88F462388C55}" name="Term Accession Number [Time point] (#h; #tNFDI4PSO:0000034)"/>
-    <tableColumn id="9" xr3:uid="{C026D2FA-5682-9149-AC82-04C41D7B2A35}" name="Parameter [Sample Collection Method]" dataDxfId="38"/>
+    <tableColumn id="9" xr3:uid="{C026D2FA-5682-9149-AC82-04C41D7B2A35}" name="Parameter [Sample Collection Method]" dataDxfId="43"/>
     <tableColumn id="10" xr3:uid="{D941A2F0-70D1-6C43-B8E4-312D00FBC1AF}" name="Term Source REF [Sample Collection Method] (#h; #tNFDI4PSO:0000009)"/>
     <tableColumn id="11" xr3:uid="{E996793A-7869-6E43-BBF7-8E316353182D}" name="Term Accession Number [Sample Collection Method] (#h; #tNFDI4PSO:0000009)"/>
-    <tableColumn id="6" xr3:uid="{C9BC9BDC-FC2A-0649-99AC-37AD60C975BE}" name="Parameter [Metabolism quenching method]" dataDxfId="37"/>
+    <tableColumn id="6" xr3:uid="{C9BC9BDC-FC2A-0649-99AC-37AD60C975BE}" name="Parameter [Metabolism quenching method]" dataDxfId="42"/>
     <tableColumn id="7" xr3:uid="{C63F9921-4A1B-8846-9A45-C9E15C349045}" name="Term Source REF [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)"/>
     <tableColumn id="8" xr3:uid="{6B1A2C09-E50D-5740-A19D-B0A918C31A36}" name="Term Accession Number [Metabolism quenching method] (#h; #tNFDI4PSO:0000010)"/>
-    <tableColumn id="3" xr3:uid="{375D5F86-ACEB-FC46-A859-5FB2E05B07A4}" name="Parameter [Sample storage]" dataDxfId="36"/>
+    <tableColumn id="3" xr3:uid="{375D5F86-ACEB-FC46-A859-5FB2E05B07A4}" name="Parameter [Sample storage]" dataDxfId="41"/>
     <tableColumn id="4" xr3:uid="{B3796990-7386-7C46-BA0A-C413229AB88B}" name="Term Source REF [Sample storage] (#h; #tNFDI4PSO:0000011)"/>
     <tableColumn id="5" xr3:uid="{2F847152-D664-6A41-80F9-F425EC32AAC2}" name="Term Accession Number [Sample storage] (#h; #tNFDI4PSO:0000011)"/>
     <tableColumn id="2" xr3:uid="{0F73B156-4484-494D-BC0D-D7598ADFA51B}" name="Sample Name"/>
@@ -1830,28 +2036,28 @@
   <autoFilter ref="A2:Z8" xr:uid="{2D1A5E86-9F30-F342-AAC5-74D248332107}"/>
   <tableColumns count="26">
     <tableColumn id="1" xr3:uid="{D2E85E1D-0D75-E04D-A53E-E65E938F2650}" name="Source Name"/>
-    <tableColumn id="24" xr3:uid="{208C2E14-8096-B846-A832-BEDB36668B54}" name="Parameter [Bio entity]" dataDxfId="35"/>
+    <tableColumn id="24" xr3:uid="{208C2E14-8096-B846-A832-BEDB36668B54}" name="Parameter [Bio entity]" dataDxfId="40"/>
     <tableColumn id="25" xr3:uid="{F635E6BA-6B6C-D94D-B8EF-0B10DFF8B39C}" name="Term Source REF [Bio entity] (#h; #tNFDI4PSO:0000012)"/>
     <tableColumn id="26" xr3:uid="{792E8FBF-4055-3E49-9B43-F4421C31E679}" name="Term Accession Number [Bio entity] (#h; #tNFDI4PSO:0000012)"/>
-    <tableColumn id="18" xr3:uid="{1582B2A7-083F-E042-AE92-B5EC2C558AA5}" name="Parameter [Biosource amount]" dataDxfId="34"/>
+    <tableColumn id="18" xr3:uid="{1582B2A7-083F-E042-AE92-B5EC2C558AA5}" name="Parameter [Biosource amount]" dataDxfId="39"/>
     <tableColumn id="19" xr3:uid="{B8A822D7-D91A-2343-9C8E-67885CD07D65}" name="Term Source REF [Biosource amount] (#h; #tNFDI4PSO:0000013)"/>
     <tableColumn id="20" xr3:uid="{F9F5ADA6-2D63-D942-97EC-CB264CBD7297}" name="Term Accession Number [Biosource amount] (#h; #tNFDI4PSO:0000013)"/>
     <tableColumn id="21" xr3:uid="{5E2BD7A3-2EB9-9F40-86D9-8442BB7BC0B2}" name="Unit [milligram] (#h; #tUO:0000022; #u)"/>
     <tableColumn id="22" xr3:uid="{E2212F4B-7282-4B43-A426-E201013BDE27}" name="Term Source REF [milligram] (#h; #tUO:0000022; #u)"/>
     <tableColumn id="23" xr3:uid="{EE8C4B86-2312-DC45-AC0D-EF661297A585}" name="Term Accession Number [milligram] (#h; #tUO:0000022; #u)"/>
-    <tableColumn id="15" xr3:uid="{67666069-E9C7-CE4C-B8B3-C56EAA5F628E}" name="Parameter [Extraction method]" dataDxfId="33"/>
+    <tableColumn id="15" xr3:uid="{67666069-E9C7-CE4C-B8B3-C56EAA5F628E}" name="Parameter [Extraction method]" dataDxfId="38"/>
     <tableColumn id="16" xr3:uid="{1C2182D2-3284-7A47-81C0-411B8A805FE7}" name="Term Source REF [Extraction method] (#h; #tNFDI4PSO:0000054)"/>
     <tableColumn id="17" xr3:uid="{0CA2072C-A4E5-9641-8EA8-EFD99AD5CE53}" name="Term Accession Number [Extraction method] (#h; #tNFDI4PSO:0000054)"/>
-    <tableColumn id="12" xr3:uid="{54EE5C68-575C-0944-A0C5-113D86849808}" name="Parameter [Extraction buffer]" dataDxfId="32"/>
+    <tableColumn id="12" xr3:uid="{54EE5C68-575C-0944-A0C5-113D86849808}" name="Parameter [Extraction buffer]" dataDxfId="37"/>
     <tableColumn id="13" xr3:uid="{7D0E608F-0F9E-234E-81BD-14EE4DE2D9D0}" name="Term Source REF [Extraction buffer] (#h; #tNFDI4PSO:0000050)"/>
     <tableColumn id="14" xr3:uid="{AF0CEAD3-C9E1-7E4D-AD32-32D0A6BF0447}" name="Term Accession Number [Extraction buffer] (#h; #tNFDI4PSO:0000050)"/>
-    <tableColumn id="6" xr3:uid="{690980D7-DB47-B342-A7FA-DBD260B8A3A5}" name="Parameter [Extraction buffer volume]" dataDxfId="31"/>
+    <tableColumn id="6" xr3:uid="{690980D7-DB47-B342-A7FA-DBD260B8A3A5}" name="Parameter [Extraction buffer volume]" dataDxfId="36"/>
     <tableColumn id="7" xr3:uid="{7442F9A1-4AB7-AE4A-AC01-CA233181C7F8}" name="Term Source REF [Extraction buffer volume] (#h; #tNFDI4PSO:0000051)"/>
     <tableColumn id="8" xr3:uid="{2A2F1DA5-C648-C242-BBE4-D46E04DC3A13}" name="Term Accession Number [Extraction buffer volume] (#h; #tNFDI4PSO:0000051)"/>
     <tableColumn id="9" xr3:uid="{3BE00BD6-C7CB-5B46-B45A-F11A99ED124A}" name="Unit [microliter] (#h; #tUO:0000101; #u)"/>
     <tableColumn id="10" xr3:uid="{FD49A6E5-9A8A-D148-A557-561579CA7940}" name="Term Source REF [microliter] (#h; #tUO:0000101; #u)"/>
     <tableColumn id="11" xr3:uid="{4F5F45D5-9F77-F544-8761-D114AA524502}" name="Term Accession Number [microliter] (#h; #tUO:0000101; #u)"/>
-    <tableColumn id="3" xr3:uid="{F4368773-8BEA-E94C-BF8F-DA78C490AECA}" name="Parameter [RNA quality check]" dataDxfId="30"/>
+    <tableColumn id="3" xr3:uid="{F4368773-8BEA-E94C-BF8F-DA78C490AECA}" name="Parameter [RNA quality check]" dataDxfId="1"/>
     <tableColumn id="4" xr3:uid="{8A909FA8-98B2-F146-968B-7D12F64864AB}" name="Term Source REF [RNA quality check] (#h; #tNFDI4PSO:0000062)"/>
     <tableColumn id="5" xr3:uid="{6FBA3FA8-17DB-F640-B15E-7947CCF3C933}" name="Term Accession Number [RNA quality check] (#h; #tNFDI4PSO:0000062)"/>
     <tableColumn id="2" xr3:uid="{C2AC46EF-7A21-2C46-A396-685200DCDE85}" name="Sample Name"/>
@@ -1861,101 +2067,99 @@
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5E50D53B-7C2E-4847-BD9B-C8D479DB11BC}" name="annotationTable2" displayName="annotationTable2" ref="A2:AY8" totalsRowShown="0">
-  <autoFilter ref="A2:AY8" xr:uid="{5E50D53B-7C2E-4847-BD9B-C8D479DB11BC}"/>
-  <tableColumns count="51">
-    <tableColumn id="1" xr3:uid="{3C0BD8C6-C13B-4342-A220-05A09CD41E28}" name="Source Name" dataDxfId="3"/>
-    <tableColumn id="49" xr3:uid="{B2A1D485-66A2-484B-87EF-F298A397CB62}" name="Parameter [Library strategy]" dataDxfId="29"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{5E50D53B-7C2E-4847-BD9B-C8D479DB11BC}" name="annotationTable2" displayName="annotationTable2" ref="A2:AX8" totalsRowShown="0">
+  <autoFilter ref="A2:AX8" xr:uid="{5E50D53B-7C2E-4847-BD9B-C8D479DB11BC}"/>
+  <tableColumns count="50">
+    <tableColumn id="1" xr3:uid="{3C0BD8C6-C13B-4342-A220-05A09CD41E28}" name="Sample Name" dataDxfId="35"/>
+    <tableColumn id="49" xr3:uid="{B2A1D485-66A2-484B-87EF-F298A397CB62}" name="Parameter [Library strategy]" dataDxfId="34"/>
     <tableColumn id="50" xr3:uid="{64B5199C-F533-6D48-B081-09445114CCDF}" name="Term Source REF [Library strategy] (#h; #tNFDI4PSO:0000035)"/>
     <tableColumn id="51" xr3:uid="{277F6EEA-6FE3-DC48-8E09-6A12B94E2D26}" name="Term Accession Number [Library strategy] (#h; #tNFDI4PSO:0000035)"/>
-    <tableColumn id="46" xr3:uid="{7634B482-A6B2-0B4E-A088-23F8A663E757}" name="Parameter [Library Selection]" dataDxfId="28"/>
+    <tableColumn id="46" xr3:uid="{7634B482-A6B2-0B4E-A088-23F8A663E757}" name="Parameter [Library Selection]" dataDxfId="33"/>
     <tableColumn id="47" xr3:uid="{7BC02BD5-8666-DA4D-8C08-62122F122DAE}" name="Term Source REF [Library Selection] (#h; #tNFDI4PSO:0000036)"/>
     <tableColumn id="48" xr3:uid="{39181008-FA88-B64E-AF89-4EE8CE16DACD}" name="Term Accession Number [Library Selection] (#h; #tNFDI4PSO:0000036)"/>
-    <tableColumn id="43" xr3:uid="{9E093EBB-26BB-C44C-B8D3-C21415747449}" name="Parameter [Library layout]" dataDxfId="27"/>
+    <tableColumn id="43" xr3:uid="{9E093EBB-26BB-C44C-B8D3-C21415747449}" name="Parameter [Library layout]" dataDxfId="32"/>
     <tableColumn id="44" xr3:uid="{30098CB4-D4E7-B54C-90D7-9966235A116F}" name="Term Source REF [Library layout] (#h; #t)"/>
     <tableColumn id="45" xr3:uid="{2821B40E-FABE-5441-9408-160FA4849433}" name="Term Accession Number [Library layout] (#h; #t)"/>
-    <tableColumn id="40" xr3:uid="{1025AAF1-1835-1643-8669-494E122B1BB7}" name="rRNA Depletion" dataDxfId="26"/>
+    <tableColumn id="40" xr3:uid="{1025AAF1-1835-1643-8669-494E122B1BB7}" name="rRNA Depletion" dataDxfId="31"/>
     <tableColumn id="41" xr3:uid="{274B99B9-6FDE-F746-930D-EA397239BD4E}" name="Term Source REF [rRNA Depletion] (#h)"/>
     <tableColumn id="42" xr3:uid="{4F5306FE-DC99-7C4D-9D5C-CA46EB6CFDAE}" name="Term Accession Number [rRNA Depletion] (#h)"/>
-    <tableColumn id="37" xr3:uid="{012C0365-268D-F14F-A056-378DBAC69A56}" name="Parameter [Library preparation kit]" dataDxfId="25"/>
+    <tableColumn id="37" xr3:uid="{012C0365-268D-F14F-A056-378DBAC69A56}" name="Parameter [Library preparation kit]" dataDxfId="30"/>
     <tableColumn id="38" xr3:uid="{F9CB580A-6FD8-D541-B732-1CE6F3C07FEA}" name="Term Source REF [Library preparation kit] (#h; #tNFDI4PSO:0000037)"/>
     <tableColumn id="39" xr3:uid="{A5F05C06-2AB8-B944-8498-53314314553A}" name="Term Accession Number [Library preparation kit] (#h; #tNFDI4PSO:0000037)"/>
-    <tableColumn id="34" xr3:uid="{1F296589-5898-A04B-BA63-1E29EE8D9067}" name="Parameter [Library preparation kit version]" dataDxfId="24"/>
+    <tableColumn id="34" xr3:uid="{1F296589-5898-A04B-BA63-1E29EE8D9067}" name="Parameter [Library preparation kit version]" dataDxfId="29"/>
     <tableColumn id="35" xr3:uid="{69530ED6-BA43-B745-855A-10BEAB4D003C}" name="Term Source REF [Library preparation kit version] (#h; #tNFDI4PSO:0000038)"/>
     <tableColumn id="36" xr3:uid="{BB141419-A75D-1645-9E91-4E794AA3B187}" name="Term Accession Number [Library preparation kit version] (#h; #tNFDI4PSO:0000038)"/>
-    <tableColumn id="31" xr3:uid="{357F1346-44A0-F24A-AC0E-6E0D3E5772ED}" name="Parameter [Adapter sequence]" dataDxfId="23"/>
+    <tableColumn id="31" xr3:uid="{357F1346-44A0-F24A-AC0E-6E0D3E5772ED}" name="Parameter [Adapter sequence]" dataDxfId="0"/>
     <tableColumn id="32" xr3:uid="{EFE2EE97-9DFD-6F4F-8420-2018D3CE6956}" name="Term Source REF [Adapter sequence] (#h; #tNFDI4PSO:0000039)"/>
     <tableColumn id="33" xr3:uid="{27C1ACDA-D124-E349-8B62-53BCF7C17C19}" name="Term Accession Number [Adapter sequence] (#h; #tNFDI4PSO:0000039)"/>
-    <tableColumn id="25" xr3:uid="{15CD417E-B011-1C4E-A7B0-2165F5087E7C}" name="Parameter [Library RNA amount]" dataDxfId="22"/>
+    <tableColumn id="25" xr3:uid="{15CD417E-B011-1C4E-A7B0-2165F5087E7C}" name="Parameter [Library RNA amount]" dataDxfId="28"/>
     <tableColumn id="26" xr3:uid="{1C411B5E-1007-E44F-A9C5-40C5E553C686}" name="Term Source REF [Library RNA amount] (#h; #tNFDI4PSO:0000016)"/>
     <tableColumn id="27" xr3:uid="{E6980BB7-47F0-B440-B608-BFA310580009}" name="Term Accession Number [Library RNA amount] (#h; #tNFDI4PSO:0000016)"/>
     <tableColumn id="28" xr3:uid="{6ABA1A9E-3D34-F841-8202-6F34F1E2E053}" name="Unit [microgram] (#h; #tUO:0000023; #u)"/>
     <tableColumn id="29" xr3:uid="{94834A38-2ED9-4743-9CA3-05766ED0ACD2}" name="Term Source REF [microgram] (#h; #tUO:0000023; #u)"/>
     <tableColumn id="30" xr3:uid="{72BA7A4C-58FD-2541-886C-88F7200CFCC2}" name="Term Accession Number [microgram] (#h; #tUO:0000023; #u)"/>
-    <tableColumn id="22" xr3:uid="{51EECCA6-8B96-6449-9E61-A7758FD15528}" name="Parameter [Next generation sequencing instrument model]" dataDxfId="21"/>
+    <tableColumn id="22" xr3:uid="{51EECCA6-8B96-6449-9E61-A7758FD15528}" name="Parameter [Next generation sequencing instrument model]" dataDxfId="27"/>
     <tableColumn id="23" xr3:uid="{6EEC8899-ED93-EF4D-ACB9-51308D7708F3}" name="Term Source REF [Next generation sequencing instrument model] (#h; #tNFDI4PSO:0000040)"/>
     <tableColumn id="24" xr3:uid="{AA47DA85-8160-ED41-83BD-5B70487FF280}" name="Term Accession Number [Next generation sequencing instrument model] (#h; #tNFDI4PSO:0000040)"/>
-    <tableColumn id="19" xr3:uid="{9FD8E609-10AF-3A44-84F5-5B86D61D02CA}" name="Parameter [Base-calling Software]" dataDxfId="20"/>
+    <tableColumn id="19" xr3:uid="{9FD8E609-10AF-3A44-84F5-5B86D61D02CA}" name="Parameter [Base-calling Software]" dataDxfId="26"/>
     <tableColumn id="20" xr3:uid="{2A69BD54-750E-1340-A97D-3CDDE196F231}" name="Term Source REF [Base-calling Software] (#h; #tNFDI4PSO:0000017)"/>
     <tableColumn id="21" xr3:uid="{2ECF6F98-8CB2-9C46-81BB-50268FBEF9E3}" name="Term Accession Number [Base-calling Software] (#h; #tNFDI4PSO:0000017)"/>
-    <tableColumn id="16" xr3:uid="{52F1F237-7D3D-544D-8679-A36838508419}" name="Parameter [Base-calling Software Version]" dataDxfId="19"/>
+    <tableColumn id="16" xr3:uid="{52F1F237-7D3D-544D-8679-A36838508419}" name="Parameter [Base-calling Software Version]" dataDxfId="25"/>
     <tableColumn id="17" xr3:uid="{235F846C-2DEF-954A-94F7-8BB79F2C6F1F}" name="Term Source REF [Base-calling Software Version] (#h; #tNFDI4PSO:0000018)"/>
     <tableColumn id="18" xr3:uid="{88250BB1-BFC1-154F-970F-78EB755C8825}" name="Term Accession Number [Base-calling Software Version] (#h; #tNFDI4PSO:0000018)"/>
-    <tableColumn id="13" xr3:uid="{A2A643D3-EFE5-F34E-8B9D-D3020399A6CA}" name="Parameter [Base-calling Software Parameters]" dataDxfId="18"/>
+    <tableColumn id="13" xr3:uid="{A2A643D3-EFE5-F34E-8B9D-D3020399A6CA}" name="Parameter [Base-calling Software Parameters]" dataDxfId="24"/>
     <tableColumn id="14" xr3:uid="{B561C897-653A-9B45-8372-384F5592122E}" name="Term Source REF [Base-calling Software Parameters] (#h; #tNFDI4PSO:0000019)"/>
     <tableColumn id="15" xr3:uid="{83F152E8-F2F8-2F44-9C25-E5A0C4CAF379}" name="Term Accession Number [Base-calling Software Parameters] (#h; #tNFDI4PSO:0000019)"/>
-    <tableColumn id="10" xr3:uid="{2E615A5C-7E61-EB4D-9BCC-3F59FDA5F531}" name="Parameter [Library strand]" dataDxfId="17"/>
+    <tableColumn id="10" xr3:uid="{2E615A5C-7E61-EB4D-9BCC-3F59FDA5F531}" name="Parameter [Library strand]" dataDxfId="23"/>
     <tableColumn id="11" xr3:uid="{74AD09BD-2022-614C-8200-E87C67DF4979}" name="Term Source REF [Library strand] (#h; #tNFDI4PSO:0000020)"/>
     <tableColumn id="12" xr3:uid="{471BADE9-140D-844C-A8E1-5F926EDECD75}" name="Term Accession Number [Library strand] (#h; #tNFDI4PSO:0000020)"/>
-    <tableColumn id="9" xr3:uid="{E53D534D-7DEA-2746-AD20-5F120888FD81}" name="Data File Name" dataDxfId="16"/>
-    <tableColumn id="6" xr3:uid="{0CA8855E-B6C2-434C-A89B-DF38AA6F9DE8}" name="Parameter [Raw data file format]" dataDxfId="15"/>
+    <tableColumn id="9" xr3:uid="{E53D534D-7DEA-2746-AD20-5F120888FD81}" name="Data File Name" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{0CA8855E-B6C2-434C-A89B-DF38AA6F9DE8}" name="Parameter [Raw data file format]" dataDxfId="21"/>
     <tableColumn id="7" xr3:uid="{42D583A5-58DA-7B42-A558-309F4C8595C9}" name="Term Source REF [Raw data file format] (#h; #tNFDI4PSO:0000021)"/>
     <tableColumn id="8" xr3:uid="{106B5C76-91C5-744D-A138-708A934821D9}" name="Term Accession Number [Raw data file format] (#h; #tNFDI4PSO:0000021)"/>
-    <tableColumn id="3" xr3:uid="{E89DE330-E700-3E45-8FAC-304E30A88A1F}" name="Parameter [Raw data file checksum]" dataDxfId="14"/>
+    <tableColumn id="3" xr3:uid="{E89DE330-E700-3E45-8FAC-304E30A88A1F}" name="Parameter [Raw data file checksum]" dataDxfId="20"/>
     <tableColumn id="4" xr3:uid="{EE368D00-3868-AC45-8363-30C114F2A9BA}" name="Term Source REF [Raw data file checksum] (#h; #tNFDI4PSO:0000022)"/>
     <tableColumn id="5" xr3:uid="{FDB8F7B5-CA34-4E4D-A06B-113844208504}" name="Term Accession Number [Raw data file checksum] (#h; #tNFDI4PSO:0000022)"/>
-    <tableColumn id="2" xr3:uid="{051F1C24-3715-614E-8F91-8A3653CEE814}" name="Sample Name" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F95E6E3D-A9BC-BA49-BEDB-35F89BAB44DD}" name="annotationTable3" displayName="annotationTable3" ref="A2:AF8" totalsRowShown="0">
-  <autoFilter ref="A2:AF8" xr:uid="{F95E6E3D-A9BC-BA49-BEDB-35F89BAB44DD}"/>
-  <tableColumns count="32">
-    <tableColumn id="1" xr3:uid="{F2D30A3B-127F-904A-9A08-B802DA5CB9EC}" name="Source Name" dataDxfId="1"/>
-    <tableColumn id="30" xr3:uid="{2F768328-C794-734B-BA79-8EE4E9619326}" name="Parameter [Data filtering software]" dataDxfId="13"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{F95E6E3D-A9BC-BA49-BEDB-35F89BAB44DD}" name="annotationTable3" displayName="annotationTable3" ref="A2:AE8" totalsRowShown="0">
+  <autoFilter ref="A2:AE8" xr:uid="{F95E6E3D-A9BC-BA49-BEDB-35F89BAB44DD}"/>
+  <tableColumns count="31">
+    <tableColumn id="33" xr3:uid="{92889B6D-15C4-C34F-A49A-CFE38371FED1}" name="Data File Name" dataDxfId="8"/>
+    <tableColumn id="30" xr3:uid="{2F768328-C794-734B-BA79-8EE4E9619326}" name="Parameter [Data filtering software]" dataDxfId="19"/>
     <tableColumn id="31" xr3:uid="{E814E128-AF78-3D4B-BD43-BC75E11F125D}" name="Term Source REF [Data filtering software] (#h; #tNFDI4PSO:0000023)"/>
     <tableColumn id="32" xr3:uid="{A39924B4-E4CB-3F44-B0FF-A5DC5F1C8FB5}" name="Term Accession Number [Data filtering software] (#h; #tNFDI4PSO:0000023)"/>
-    <tableColumn id="27" xr3:uid="{DE60A512-17C1-664E-A0B4-8E2FAE917A15}" name="Parameter [Data filtering software version]" dataDxfId="12"/>
+    <tableColumn id="27" xr3:uid="{DE60A512-17C1-664E-A0B4-8E2FAE917A15}" name="Parameter [Data filtering software version]" dataDxfId="18"/>
     <tableColumn id="28" xr3:uid="{3D078A49-ECD4-9C43-B71A-679D624D7F32}" name="Term Source REF [Data filtering software version] (#h; #tNFDI4PSO:0000024)"/>
     <tableColumn id="29" xr3:uid="{5B75A048-CB4F-434B-A6D8-E0BDCCD691C7}" name="Term Accession Number [Data filtering software version] (#h; #tNFDI4PSO:0000024)"/>
-    <tableColumn id="24" xr3:uid="{0268DADC-BE98-DE4B-8C44-E97693119BA6}" name="Parameter [Data filtering Software Parameters]" dataDxfId="11"/>
+    <tableColumn id="24" xr3:uid="{0268DADC-BE98-DE4B-8C44-E97693119BA6}" name="Parameter [Data filtering Software Parameters]" dataDxfId="17"/>
     <tableColumn id="25" xr3:uid="{2BE975C3-7C90-8245-8215-CABAB93A5DAF}" name="Term Source REF [Data filtering Software Parameters] (#h; #tNFDI4PSO:0000025)"/>
     <tableColumn id="26" xr3:uid="{61FACAFC-4E6A-6B40-836E-BDE261E57CD8}" name="Term Accession Number [Data filtering Software Parameters] (#h; #tNFDI4PSO:0000025)"/>
-    <tableColumn id="21" xr3:uid="{690D0F48-A963-924F-B797-3FA04E2C4FF7}" name="Parameter [Read Alignment Software]" dataDxfId="10"/>
+    <tableColumn id="21" xr3:uid="{690D0F48-A963-924F-B797-3FA04E2C4FF7}" name="Parameter [Read Alignment Software]" dataDxfId="16"/>
     <tableColumn id="22" xr3:uid="{5019C456-5FF6-824B-A278-816252676424}" name="Term Source REF [Read Alignment Software] (#h; #tNFDI4PSO:0000002)"/>
     <tableColumn id="23" xr3:uid="{09CD7A74-EBC4-944E-A3A0-B3D3EE0F223B}" name="Term Accession Number [Read Alignment Software] (#h; #tNFDI4PSO:0000002)"/>
-    <tableColumn id="18" xr3:uid="{BCDCB4C1-F1B1-FF46-935C-3A63FF2AEBD6}" name="Parameter [Read Alignment Software Version]" dataDxfId="9"/>
+    <tableColumn id="18" xr3:uid="{BCDCB4C1-F1B1-FF46-935C-3A63FF2AEBD6}" name="Parameter [Read Alignment Software Version]" dataDxfId="15"/>
     <tableColumn id="19" xr3:uid="{DCFAB53F-6C7F-A143-AFEF-883C72A296F2}" name="Term Source REF [Read Alignment Software Version] (#h; #tNFDI4PSO:0000003)"/>
     <tableColumn id="20" xr3:uid="{57FE72CC-6B5E-E34D-AA54-3018DC881474}" name="Term Accession Number [Read Alignment Software Version] (#h; #tNFDI4PSO:0000003)"/>
-    <tableColumn id="15" xr3:uid="{4B6756EB-DBB4-454F-9F88-C0BDFB279D45}" name="Parameter [Read Alignment Software Parameters]" dataDxfId="8"/>
+    <tableColumn id="15" xr3:uid="{4B6756EB-DBB4-454F-9F88-C0BDFB279D45}" name="Parameter [Read Alignment Software Parameters]" dataDxfId="14"/>
     <tableColumn id="16" xr3:uid="{AB7F1A22-7B59-0143-9EA8-776293BA81EE}" name="Term Source REF [Read Alignment Software Parameters] (#h; #tNFDI4PSO:0000004)"/>
     <tableColumn id="17" xr3:uid="{EFC6E5B4-6B00-D54E-A0C7-E9B2332AA565}" name="Term Accession Number [Read Alignment Software Parameters] (#h; #tNFDI4PSO:0000004)"/>
-    <tableColumn id="12" xr3:uid="{8F865758-F7B1-8B4F-8BAF-140E6BAD82C3}" name="Parameter [Genome reference sequence]" dataDxfId="7"/>
+    <tableColumn id="12" xr3:uid="{8F865758-F7B1-8B4F-8BAF-140E6BAD82C3}" name="Parameter [Genome reference sequence]" dataDxfId="13"/>
     <tableColumn id="13" xr3:uid="{CFBF4F52-5533-3E4D-A77D-8670D665242E}" name="Term Source REF [Genome reference sequence] (#h; #tNFDI4PSO:0000026)"/>
     <tableColumn id="14" xr3:uid="{1E199F8C-B5BA-FB4E-8F36-9A907E2472B9}" name="Term Accession Number [Genome reference sequence] (#h; #tNFDI4PSO:0000026)"/>
-    <tableColumn id="9" xr3:uid="{AD58508F-D0C5-3E48-A205-1E6F97883B1E}" name="Parameter [Processed data file name]" dataDxfId="6"/>
+    <tableColumn id="9" xr3:uid="{AD58508F-D0C5-3E48-A205-1E6F97883B1E}" name="Parameter [Processed data file name]" dataDxfId="12"/>
     <tableColumn id="10" xr3:uid="{B0BFA4E3-8EE0-1842-B7CB-5BABC14AE8DE}" name="Term Source REF [Processed data file name] (#h; #tNFDI4PSO:0000028)"/>
     <tableColumn id="11" xr3:uid="{2147C9CD-B05A-0246-9E30-CC28F82A22DB}" name="Term Accession Number [Processed data file name] (#h; #tNFDI4PSO:0000028)"/>
-    <tableColumn id="6" xr3:uid="{3CB9D074-1D94-9246-A29F-29AAD572E62D}" name="Parameter [Processed data file format]" dataDxfId="5"/>
+    <tableColumn id="6" xr3:uid="{3CB9D074-1D94-9246-A29F-29AAD572E62D}" name="Parameter [Processed data file format]" dataDxfId="11"/>
     <tableColumn id="7" xr3:uid="{AEE72515-E8F8-824D-A775-D2CBE15BCB45}" name="Term Source REF [Processed data file format] (#h; #tNFDI4PSO:0000027)"/>
     <tableColumn id="8" xr3:uid="{978F5E10-9BEA-5845-A668-55ECA92B3E69}" name="Term Accession Number [Processed data file format] (#h; #tNFDI4PSO:0000027)"/>
-    <tableColumn id="3" xr3:uid="{A5045089-5E18-4E41-A31A-E21A7A646DC7}" name="Parameter [Processed data file checksum]" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{A5045089-5E18-4E41-A31A-E21A7A646DC7}" name="Parameter [Processed data file checksum]" dataDxfId="10"/>
     <tableColumn id="4" xr3:uid="{9629D861-4EC3-4240-80EA-A3F3AAA74ACA}" name="Term Source REF [Processed data file checksum] (#h; #tNFDI4PSO:0000029)"/>
     <tableColumn id="5" xr3:uid="{4B2781B5-D387-3C48-ABE3-BBB5BE1B1998}" name="Term Accession Number [Processed data file checksum] (#h; #tNFDI4PSO:0000029)"/>
-    <tableColumn id="2" xr3:uid="{6B9EAC32-6968-9046-981D-C29FAD11BC9E}" name="Sample Name" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium7" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2276,10 +2480,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:DX8"/>
+  <dimension ref="A1:ED8"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="BY1" zoomScale="75" workbookViewId="0">
-      <selection activeCell="CQ9" sqref="CQ9"/>
+    <sheetView tabSelected="1" zoomScale="117" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2318,7 +2522,7 @@
     <col min="32" max="32" width="25" bestFit="1" customWidth="1"/>
     <col min="33" max="33" width="50.33203125" hidden="1" customWidth="1"/>
     <col min="34" max="34" width="56.5" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="20.6640625" bestFit="1" customWidth="1"/>
+    <col min="35" max="35" width="22.6640625" bestFit="1" customWidth="1"/>
     <col min="36" max="36" width="46" hidden="1" customWidth="1"/>
     <col min="37" max="37" width="52.1640625" hidden="1" customWidth="1"/>
     <col min="38" max="38" width="36" bestFit="1" customWidth="1"/>
@@ -2337,88 +2541,1707 @@
     <col min="51" max="51" width="50.33203125" hidden="1" customWidth="1"/>
     <col min="52" max="52" width="56.5" hidden="1" customWidth="1"/>
     <col min="53" max="53" width="26.5" bestFit="1" customWidth="1"/>
-    <col min="54" max="54" width="47.5" hidden="1" customWidth="1"/>
-    <col min="55" max="55" width="53.6640625" hidden="1" customWidth="1"/>
-    <col min="56" max="56" width="44.1640625" bestFit="1" customWidth="1"/>
-    <col min="57" max="57" width="65.33203125" hidden="1" customWidth="1"/>
-    <col min="58" max="58" width="71.5" hidden="1" customWidth="1"/>
-    <col min="59" max="59" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="60" max="60" width="58.6640625" hidden="1" customWidth="1"/>
-    <col min="61" max="61" width="64.83203125" hidden="1" customWidth="1"/>
-    <col min="62" max="62" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="63" max="63" width="58.6640625" hidden="1" customWidth="1"/>
-    <col min="64" max="64" width="64.83203125" hidden="1" customWidth="1"/>
-    <col min="65" max="65" width="37.5" bestFit="1" customWidth="1"/>
-    <col min="66" max="66" width="58.5" hidden="1" customWidth="1"/>
-    <col min="67" max="67" width="64.6640625" hidden="1" customWidth="1"/>
-    <col min="68" max="68" width="65.5" hidden="1" customWidth="1"/>
-    <col min="69" max="69" width="76.33203125" hidden="1" customWidth="1"/>
-    <col min="70" max="70" width="82.5" hidden="1" customWidth="1"/>
-    <col min="71" max="71" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="72" max="72" width="54.6640625" hidden="1" customWidth="1"/>
-    <col min="73" max="73" width="61" hidden="1" customWidth="1"/>
-    <col min="74" max="74" width="38.5" hidden="1" customWidth="1"/>
-    <col min="75" max="75" width="49.33203125" hidden="1" customWidth="1"/>
-    <col min="76" max="76" width="55.6640625" hidden="1" customWidth="1"/>
-    <col min="77" max="77" width="30.6640625" bestFit="1" customWidth="1"/>
-    <col min="78" max="78" width="56" hidden="1" customWidth="1"/>
-    <col min="79" max="79" width="62.1640625" hidden="1" customWidth="1"/>
-    <col min="80" max="80" width="35.5" hidden="1" customWidth="1"/>
-    <col min="81" max="81" width="46.33203125" hidden="1" customWidth="1"/>
-    <col min="82" max="82" width="52.5" hidden="1" customWidth="1"/>
-    <col min="83" max="83" width="32.5" bestFit="1" customWidth="1"/>
-    <col min="84" max="84" width="57.83203125" hidden="1" customWidth="1"/>
-    <col min="85" max="85" width="64" hidden="1" customWidth="1"/>
-    <col min="86" max="86" width="44.33203125" hidden="1" customWidth="1"/>
-    <col min="87" max="87" width="55.33203125" hidden="1" customWidth="1"/>
-    <col min="88" max="88" width="61.5" hidden="1" customWidth="1"/>
-    <col min="89" max="89" width="33.6640625" bestFit="1" customWidth="1"/>
-    <col min="90" max="90" width="59" hidden="1" customWidth="1"/>
-    <col min="91" max="91" width="65.33203125" hidden="1" customWidth="1"/>
-    <col min="92" max="92" width="41.33203125" hidden="1" customWidth="1"/>
-    <col min="93" max="93" width="52.1640625" hidden="1" customWidth="1"/>
-    <col min="94" max="94" width="58.33203125" hidden="1" customWidth="1"/>
-    <col min="95" max="95" width="33.33203125" bestFit="1" customWidth="1"/>
-    <col min="96" max="96" width="54.33203125" hidden="1" customWidth="1"/>
-    <col min="97" max="97" width="60.6640625" hidden="1" customWidth="1"/>
-    <col min="98" max="98" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="99" max="99" width="58.33203125" hidden="1" customWidth="1"/>
-    <col min="100" max="100" width="64.5" hidden="1" customWidth="1"/>
-    <col min="101" max="101" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="102" max="102" width="57.33203125" hidden="1" customWidth="1"/>
-    <col min="103" max="103" width="63.5" hidden="1" customWidth="1"/>
-    <col min="104" max="104" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="105" max="105" width="56.33203125" hidden="1" customWidth="1"/>
-    <col min="106" max="106" width="62.5" hidden="1" customWidth="1"/>
-    <col min="107" max="107" width="31.6640625" bestFit="1" customWidth="1"/>
-    <col min="108" max="108" width="57" hidden="1" customWidth="1"/>
-    <col min="109" max="109" width="63.1640625" hidden="1" customWidth="1"/>
-    <col min="110" max="110" width="37.33203125" bestFit="1" customWidth="1"/>
-    <col min="111" max="111" width="62.6640625" hidden="1" customWidth="1"/>
-    <col min="112" max="112" width="68.83203125" hidden="1" customWidth="1"/>
-    <col min="113" max="113" width="35" bestFit="1" customWidth="1"/>
-    <col min="114" max="114" width="60.33203125" hidden="1" customWidth="1"/>
-    <col min="115" max="115" width="66.5" hidden="1" customWidth="1"/>
-    <col min="116" max="116" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="117" max="117" width="52" hidden="1" customWidth="1"/>
-    <col min="118" max="118" width="58.1640625" hidden="1" customWidth="1"/>
-    <col min="119" max="119" width="36.33203125" bestFit="1" customWidth="1"/>
-    <col min="120" max="120" width="65" hidden="1" customWidth="1"/>
-    <col min="121" max="121" width="71.33203125" hidden="1" customWidth="1"/>
-    <col min="122" max="122" width="40.5" bestFit="1" customWidth="1"/>
-    <col min="123" max="123" width="69.1640625" hidden="1" customWidth="1"/>
-    <col min="124" max="124" width="75.33203125" hidden="1" customWidth="1"/>
-    <col min="125" max="125" width="27.33203125" bestFit="1" customWidth="1"/>
-    <col min="126" max="126" width="56.1640625" hidden="1" customWidth="1"/>
-    <col min="127" max="127" width="62.33203125" hidden="1" customWidth="1"/>
-    <col min="128" max="128" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="54" max="54" width="47.5" customWidth="1"/>
+    <col min="55" max="58" width="53.6640625" customWidth="1"/>
+    <col min="59" max="59" width="44.1640625" bestFit="1" customWidth="1"/>
+    <col min="60" max="60" width="65.33203125" hidden="1" customWidth="1"/>
+    <col min="61" max="61" width="71.5" hidden="1" customWidth="1"/>
+    <col min="62" max="63" width="38.6640625" bestFit="1" customWidth="1"/>
+    <col min="64" max="64" width="38.83203125" bestFit="1" customWidth="1"/>
+    <col min="65" max="65" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="66" max="66" width="58.6640625" hidden="1" customWidth="1"/>
+    <col min="67" max="67" width="64.83203125" hidden="1" customWidth="1"/>
+    <col min="68" max="68" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="69" max="69" width="58.6640625" hidden="1" customWidth="1"/>
+    <col min="70" max="70" width="64.83203125" hidden="1" customWidth="1"/>
+    <col min="71" max="71" width="43.33203125" bestFit="1" customWidth="1"/>
+    <col min="72" max="72" width="58.5" hidden="1" customWidth="1"/>
+    <col min="73" max="73" width="64.6640625" hidden="1" customWidth="1"/>
+    <col min="74" max="74" width="65.5" hidden="1" customWidth="1"/>
+    <col min="75" max="75" width="76.33203125" hidden="1" customWidth="1"/>
+    <col min="76" max="76" width="82.5" hidden="1" customWidth="1"/>
+    <col min="77" max="77" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="78" max="78" width="54.6640625" hidden="1" customWidth="1"/>
+    <col min="79" max="79" width="61" hidden="1" customWidth="1"/>
+    <col min="80" max="80" width="38.5" hidden="1" customWidth="1"/>
+    <col min="81" max="81" width="49.33203125" hidden="1" customWidth="1"/>
+    <col min="82" max="82" width="55.6640625" hidden="1" customWidth="1"/>
+    <col min="83" max="83" width="30.6640625" bestFit="1" customWidth="1"/>
+    <col min="84" max="84" width="56" hidden="1" customWidth="1"/>
+    <col min="85" max="85" width="62.1640625" hidden="1" customWidth="1"/>
+    <col min="86" max="86" width="35.5" hidden="1" customWidth="1"/>
+    <col min="87" max="87" width="46.33203125" hidden="1" customWidth="1"/>
+    <col min="88" max="88" width="52.5" hidden="1" customWidth="1"/>
+    <col min="89" max="89" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="90" max="90" width="57.83203125" hidden="1" customWidth="1"/>
+    <col min="91" max="91" width="64" hidden="1" customWidth="1"/>
+    <col min="92" max="92" width="44.33203125" hidden="1" customWidth="1"/>
+    <col min="93" max="93" width="55.33203125" hidden="1" customWidth="1"/>
+    <col min="94" max="94" width="61.5" hidden="1" customWidth="1"/>
+    <col min="95" max="95" width="33.6640625" bestFit="1" customWidth="1"/>
+    <col min="96" max="96" width="59" hidden="1" customWidth="1"/>
+    <col min="97" max="97" width="65.33203125" hidden="1" customWidth="1"/>
+    <col min="98" max="98" width="41.33203125" hidden="1" customWidth="1"/>
+    <col min="99" max="99" width="52.1640625" hidden="1" customWidth="1"/>
+    <col min="100" max="100" width="58.33203125" hidden="1" customWidth="1"/>
+    <col min="101" max="101" width="33.33203125" bestFit="1" customWidth="1"/>
+    <col min="102" max="102" width="54.33203125" hidden="1" customWidth="1"/>
+    <col min="103" max="103" width="60.6640625" hidden="1" customWidth="1"/>
+    <col min="104" max="104" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="105" max="105" width="58.33203125" hidden="1" customWidth="1"/>
+    <col min="106" max="106" width="64.5" hidden="1" customWidth="1"/>
+    <col min="107" max="107" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="108" max="108" width="57.33203125" hidden="1" customWidth="1"/>
+    <col min="109" max="109" width="63.5" hidden="1" customWidth="1"/>
+    <col min="110" max="110" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="111" max="111" width="56.33203125" hidden="1" customWidth="1"/>
+    <col min="112" max="112" width="62.5" hidden="1" customWidth="1"/>
+    <col min="113" max="113" width="31.6640625" bestFit="1" customWidth="1"/>
+    <col min="114" max="114" width="57" hidden="1" customWidth="1"/>
+    <col min="115" max="115" width="63.1640625" hidden="1" customWidth="1"/>
+    <col min="116" max="116" width="37.33203125" bestFit="1" customWidth="1"/>
+    <col min="117" max="117" width="62.6640625" hidden="1" customWidth="1"/>
+    <col min="118" max="118" width="68.83203125" hidden="1" customWidth="1"/>
+    <col min="119" max="119" width="35" bestFit="1" customWidth="1"/>
+    <col min="120" max="120" width="60.33203125" hidden="1" customWidth="1"/>
+    <col min="121" max="121" width="66.5" hidden="1" customWidth="1"/>
+    <col min="122" max="122" width="26.6640625" bestFit="1" customWidth="1"/>
+    <col min="123" max="123" width="52" hidden="1" customWidth="1"/>
+    <col min="124" max="124" width="58.1640625" hidden="1" customWidth="1"/>
+    <col min="125" max="125" width="36.33203125" bestFit="1" customWidth="1"/>
+    <col min="126" max="126" width="65" hidden="1" customWidth="1"/>
+    <col min="127" max="127" width="71.33203125" hidden="1" customWidth="1"/>
+    <col min="128" max="128" width="40.5" bestFit="1" customWidth="1"/>
+    <col min="129" max="129" width="69.1640625" hidden="1" customWidth="1"/>
+    <col min="130" max="130" width="75.33203125" hidden="1" customWidth="1"/>
+    <col min="131" max="131" width="27.33203125" bestFit="1" customWidth="1"/>
+    <col min="132" max="132" width="56.1640625" hidden="1" customWidth="1"/>
+    <col min="133" max="133" width="62.33203125" hidden="1" customWidth="1"/>
+    <col min="134" max="134" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:134" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
         <v>151</v>
       </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+      <c r="AF1" s="11"/>
+      <c r="AG1" s="11"/>
+      <c r="AH1" s="11"/>
+      <c r="AI1" s="11"/>
+      <c r="AJ1" s="11"/>
+      <c r="AK1" s="11"/>
+      <c r="AL1" s="11"/>
+      <c r="AM1" s="11"/>
+      <c r="AN1" s="11"/>
+      <c r="AO1" s="11"/>
+      <c r="AP1" s="11"/>
+      <c r="AQ1" s="11"/>
+      <c r="AR1" s="11"/>
+      <c r="AS1" s="11"/>
+      <c r="AT1" s="11"/>
+      <c r="AU1" s="11"/>
+      <c r="AV1" s="11"/>
+      <c r="AW1" s="11"/>
+      <c r="AX1" s="11"/>
+      <c r="AY1" s="11"/>
+      <c r="AZ1" s="11"/>
+      <c r="BA1" s="11"/>
+      <c r="BB1" s="11"/>
+      <c r="BC1" s="11"/>
+      <c r="BD1" s="11"/>
+      <c r="BE1" s="11"/>
+      <c r="BF1" s="11"/>
+      <c r="BG1" s="11"/>
+      <c r="BH1" s="11"/>
+      <c r="BI1" s="11"/>
+      <c r="BJ1" s="11"/>
+      <c r="BK1" s="11"/>
+      <c r="BL1" s="11"/>
+      <c r="BM1" s="11"/>
+      <c r="BN1" s="11"/>
+      <c r="BO1" s="11"/>
+      <c r="BP1" s="11"/>
+      <c r="BQ1" s="11"/>
+      <c r="BR1" s="11"/>
+      <c r="BS1" s="11"/>
+      <c r="BT1" s="11"/>
+      <c r="BU1" s="11"/>
+      <c r="BV1" s="11"/>
+      <c r="BW1" s="11"/>
+      <c r="BX1" s="11"/>
+      <c r="BY1" s="11"/>
+      <c r="BZ1" s="11"/>
+      <c r="CA1" s="11"/>
+      <c r="CB1" s="11"/>
+      <c r="CC1" s="11"/>
+      <c r="CD1" s="11"/>
+      <c r="CE1" s="11"/>
+      <c r="CF1" s="11"/>
+      <c r="CG1" s="11"/>
+      <c r="CH1" s="11"/>
+      <c r="CI1" s="11"/>
+      <c r="CJ1" s="11"/>
+      <c r="CK1" s="11"/>
+      <c r="CL1" s="11"/>
+      <c r="CM1" s="11"/>
+      <c r="CN1" s="11"/>
+      <c r="CO1" s="11"/>
+      <c r="CP1" s="11"/>
+      <c r="CQ1" s="11"/>
+      <c r="CR1" s="11"/>
+      <c r="CS1" s="11"/>
+      <c r="CT1" s="11"/>
+      <c r="CU1" s="11"/>
+      <c r="CV1" s="11"/>
+      <c r="CW1" s="11"/>
+      <c r="CX1" s="11"/>
+      <c r="CY1" s="11"/>
+      <c r="CZ1" s="11"/>
+      <c r="DA1" s="11"/>
+      <c r="DB1" s="11"/>
+      <c r="DC1" s="11"/>
+      <c r="DD1" s="11"/>
+      <c r="DE1" s="11"/>
+      <c r="DF1" s="11"/>
+      <c r="DG1" s="11"/>
+      <c r="DH1" s="11"/>
+      <c r="DI1" s="11"/>
+      <c r="DJ1" s="11"/>
+      <c r="DK1" s="11"/>
+      <c r="DL1" s="11"/>
+      <c r="DM1" s="11"/>
+      <c r="DN1" s="11"/>
+      <c r="DO1" s="11"/>
+      <c r="DP1" s="11"/>
+      <c r="DQ1" s="11"/>
+      <c r="DR1" s="11"/>
+      <c r="DS1" s="11"/>
+      <c r="DT1" s="11"/>
+      <c r="DU1" s="11"/>
+      <c r="DV1" s="11"/>
+      <c r="DW1" s="11"/>
+      <c r="DX1" s="11"/>
+      <c r="DY1" s="11"/>
+      <c r="DZ1" s="11"/>
+      <c r="EA1" s="11"/>
+      <c r="EB1" s="11"/>
+      <c r="EC1" s="11"/>
+      <c r="ED1" s="2"/>
+    </row>
+    <row r="2" spans="1:134" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>148</v>
+      </c>
+      <c r="C2" t="s">
+        <v>149</v>
+      </c>
+      <c r="D2" t="s">
+        <v>150</v>
+      </c>
+      <c r="E2" t="s">
+        <v>145</v>
+      </c>
+      <c r="F2" t="s">
+        <v>146</v>
+      </c>
+      <c r="G2" t="s">
+        <v>147</v>
+      </c>
+      <c r="H2" t="s">
+        <v>142</v>
+      </c>
+      <c r="I2" t="s">
+        <v>143</v>
+      </c>
+      <c r="J2" t="s">
+        <v>144</v>
+      </c>
+      <c r="K2" t="s">
+        <v>139</v>
+      </c>
+      <c r="L2" t="s">
+        <v>140</v>
+      </c>
+      <c r="M2" t="s">
+        <v>141</v>
+      </c>
+      <c r="N2" t="s">
+        <v>136</v>
+      </c>
+      <c r="O2" t="s">
+        <v>137</v>
+      </c>
+      <c r="P2" t="s">
+        <v>138</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>133</v>
+      </c>
+      <c r="R2" t="s">
+        <v>134</v>
+      </c>
+      <c r="S2" t="s">
+        <v>135</v>
+      </c>
+      <c r="T2" t="s">
+        <v>130</v>
+      </c>
+      <c r="U2" t="s">
+        <v>131</v>
+      </c>
+      <c r="V2" t="s">
+        <v>132</v>
+      </c>
+      <c r="W2" t="s">
+        <v>127</v>
+      </c>
+      <c r="X2" t="s">
+        <v>128</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>129</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>124</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>125</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>126</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>121</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>122</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>123</v>
+      </c>
+      <c r="AF2" t="s">
+        <v>118</v>
+      </c>
+      <c r="AG2" t="s">
+        <v>119</v>
+      </c>
+      <c r="AH2" t="s">
+        <v>120</v>
+      </c>
+      <c r="AI2" t="s">
+        <v>115</v>
+      </c>
+      <c r="AJ2" t="s">
+        <v>116</v>
+      </c>
+      <c r="AK2" t="s">
+        <v>117</v>
+      </c>
+      <c r="AL2" t="s">
+        <v>112</v>
+      </c>
+      <c r="AM2" t="s">
+        <v>113</v>
+      </c>
+      <c r="AN2" t="s">
+        <v>114</v>
+      </c>
+      <c r="AO2" t="s">
+        <v>109</v>
+      </c>
+      <c r="AP2" t="s">
+        <v>110</v>
+      </c>
+      <c r="AQ2" t="s">
+        <v>111</v>
+      </c>
+      <c r="AR2" t="s">
+        <v>106</v>
+      </c>
+      <c r="AS2" t="s">
+        <v>107</v>
+      </c>
+      <c r="AT2" t="s">
+        <v>108</v>
+      </c>
+      <c r="AU2" t="s">
+        <v>103</v>
+      </c>
+      <c r="AV2" t="s">
+        <v>104</v>
+      </c>
+      <c r="AW2" t="s">
+        <v>105</v>
+      </c>
+      <c r="AX2" t="s">
+        <v>100</v>
+      </c>
+      <c r="AY2" t="s">
+        <v>101</v>
+      </c>
+      <c r="AZ2" t="s">
+        <v>102</v>
+      </c>
+      <c r="BA2" t="s">
+        <v>97</v>
+      </c>
+      <c r="BB2" t="s">
+        <v>98</v>
+      </c>
+      <c r="BC2" t="s">
+        <v>99</v>
+      </c>
+      <c r="BD2" t="s">
+        <v>285</v>
+      </c>
+      <c r="BE2" t="s">
+        <v>288</v>
+      </c>
+      <c r="BF2" t="s">
+        <v>289</v>
+      </c>
+      <c r="BG2" t="s">
+        <v>94</v>
+      </c>
+      <c r="BH2" t="s">
+        <v>95</v>
+      </c>
+      <c r="BI2" t="s">
+        <v>96</v>
+      </c>
+      <c r="BJ2" t="s">
+        <v>290</v>
+      </c>
+      <c r="BK2" t="s">
+        <v>291</v>
+      </c>
+      <c r="BL2" t="s">
+        <v>292</v>
+      </c>
+      <c r="BM2" t="s">
+        <v>91</v>
+      </c>
+      <c r="BN2" t="s">
+        <v>92</v>
+      </c>
+      <c r="BO2" t="s">
+        <v>93</v>
+      </c>
+      <c r="BP2" t="s">
+        <v>88</v>
+      </c>
+      <c r="BQ2" t="s">
+        <v>89</v>
+      </c>
+      <c r="BR2" t="s">
+        <v>90</v>
+      </c>
+      <c r="BS2" t="s">
+        <v>82</v>
+      </c>
+      <c r="BT2" t="s">
+        <v>83</v>
+      </c>
+      <c r="BU2" t="s">
+        <v>84</v>
+      </c>
+      <c r="BV2" t="s">
+        <v>85</v>
+      </c>
+      <c r="BW2" t="s">
+        <v>86</v>
+      </c>
+      <c r="BX2" t="s">
+        <v>87</v>
+      </c>
+      <c r="BY2" t="s">
+        <v>76</v>
+      </c>
+      <c r="BZ2" t="s">
+        <v>77</v>
+      </c>
+      <c r="CA2" t="s">
+        <v>78</v>
+      </c>
+      <c r="CB2" t="s">
+        <v>79</v>
+      </c>
+      <c r="CC2" t="s">
+        <v>80</v>
+      </c>
+      <c r="CD2" t="s">
+        <v>81</v>
+      </c>
+      <c r="CE2" t="s">
+        <v>70</v>
+      </c>
+      <c r="CF2" t="s">
+        <v>71</v>
+      </c>
+      <c r="CG2" t="s">
+        <v>72</v>
+      </c>
+      <c r="CH2" t="s">
+        <v>73</v>
+      </c>
+      <c r="CI2" t="s">
+        <v>74</v>
+      </c>
+      <c r="CJ2" t="s">
+        <v>75</v>
+      </c>
+      <c r="CK2" t="s">
+        <v>64</v>
+      </c>
+      <c r="CL2" t="s">
+        <v>65</v>
+      </c>
+      <c r="CM2" t="s">
+        <v>66</v>
+      </c>
+      <c r="CN2" t="s">
+        <v>67</v>
+      </c>
+      <c r="CO2" t="s">
+        <v>68</v>
+      </c>
+      <c r="CP2" t="s">
+        <v>69</v>
+      </c>
+      <c r="CQ2" t="s">
+        <v>58</v>
+      </c>
+      <c r="CR2" t="s">
+        <v>59</v>
+      </c>
+      <c r="CS2" t="s">
+        <v>60</v>
+      </c>
+      <c r="CT2" t="s">
+        <v>61</v>
+      </c>
+      <c r="CU2" t="s">
+        <v>62</v>
+      </c>
+      <c r="CV2" t="s">
+        <v>63</v>
+      </c>
+      <c r="CW2" t="s">
+        <v>55</v>
+      </c>
+      <c r="CX2" t="s">
+        <v>56</v>
+      </c>
+      <c r="CY2" t="s">
+        <v>57</v>
+      </c>
+      <c r="CZ2" t="s">
+        <v>52</v>
+      </c>
+      <c r="DA2" t="s">
+        <v>53</v>
+      </c>
+      <c r="DB2" t="s">
+        <v>54</v>
+      </c>
+      <c r="DC2" t="s">
+        <v>49</v>
+      </c>
+      <c r="DD2" t="s">
+        <v>50</v>
+      </c>
+      <c r="DE2" t="s">
+        <v>51</v>
+      </c>
+      <c r="DF2" t="s">
+        <v>46</v>
+      </c>
+      <c r="DG2" t="s">
+        <v>47</v>
+      </c>
+      <c r="DH2" t="s">
+        <v>48</v>
+      </c>
+      <c r="DI2" t="s">
+        <v>43</v>
+      </c>
+      <c r="DJ2" t="s">
+        <v>44</v>
+      </c>
+      <c r="DK2" t="s">
+        <v>45</v>
+      </c>
+      <c r="DL2" t="s">
+        <v>40</v>
+      </c>
+      <c r="DM2" t="s">
+        <v>41</v>
+      </c>
+      <c r="DN2" t="s">
+        <v>42</v>
+      </c>
+      <c r="DO2" t="s">
+        <v>37</v>
+      </c>
+      <c r="DP2" t="s">
+        <v>38</v>
+      </c>
+      <c r="DQ2" t="s">
+        <v>39</v>
+      </c>
+      <c r="DR2" t="s">
+        <v>34</v>
+      </c>
+      <c r="DS2" t="s">
+        <v>35</v>
+      </c>
+      <c r="DT2" t="s">
+        <v>36</v>
+      </c>
+      <c r="DU2" t="s">
+        <v>31</v>
+      </c>
+      <c r="DV2" t="s">
+        <v>32</v>
+      </c>
+      <c r="DW2" t="s">
+        <v>33</v>
+      </c>
+      <c r="DX2" t="s">
+        <v>28</v>
+      </c>
+      <c r="DY2" t="s">
+        <v>29</v>
+      </c>
+      <c r="DZ2" t="s">
+        <v>30</v>
+      </c>
+      <c r="EA2" t="s">
+        <v>25</v>
+      </c>
+      <c r="EB2" t="s">
+        <v>26</v>
+      </c>
+      <c r="EC2" t="s">
+        <v>27</v>
+      </c>
+      <c r="ED2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:134" x14ac:dyDescent="0.2">
+      <c r="A3" s="12" t="s">
+        <v>275</v>
+      </c>
+      <c r="B3" s="3"/>
+      <c r="E3" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="K3" s="3"/>
+      <c r="N3" s="3"/>
+      <c r="Q3" s="3"/>
+      <c r="T3" s="3"/>
+      <c r="W3" s="3"/>
+      <c r="Z3" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AC3" s="3"/>
+      <c r="AF3" s="3"/>
+      <c r="AI3" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="AK3" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL3" s="3"/>
+      <c r="AO3" s="3"/>
+      <c r="AR3" s="3"/>
+      <c r="AU3" s="3"/>
+      <c r="AX3" s="3"/>
+      <c r="BA3" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="BB3" t="s">
+        <v>283</v>
+      </c>
+      <c r="BC3" t="s">
+        <v>284</v>
+      </c>
+      <c r="BD3" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="BE3" s="3"/>
+      <c r="BF3" s="3"/>
+      <c r="BG3" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="BJ3" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="BK3" s="3"/>
+      <c r="BL3" s="3"/>
+      <c r="BM3" s="3"/>
+      <c r="BP3" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="BS3" s="4">
+        <v>425</v>
+      </c>
+      <c r="BT3" s="4">
+        <v>425</v>
+      </c>
+      <c r="BU3" s="4">
+        <v>425</v>
+      </c>
+      <c r="BV3" s="4">
+        <v>425</v>
+      </c>
+      <c r="BW3" s="4">
+        <v>425</v>
+      </c>
+      <c r="BX3" s="4">
+        <v>425</v>
+      </c>
+      <c r="BY3" s="5">
+        <v>37</v>
+      </c>
+      <c r="CE3" s="5">
+        <v>37</v>
+      </c>
+      <c r="CF3" s="5">
+        <v>37</v>
+      </c>
+      <c r="CG3" s="5">
+        <v>37</v>
+      </c>
+      <c r="CH3" s="5">
+        <v>37</v>
+      </c>
+      <c r="CI3" s="5">
+        <v>37</v>
+      </c>
+      <c r="CJ3" s="5">
+        <v>37</v>
+      </c>
+      <c r="CK3" s="6">
+        <v>30</v>
+      </c>
+      <c r="CQ3" s="6">
+        <v>22</v>
+      </c>
+      <c r="CR3" s="6">
+        <v>22</v>
+      </c>
+      <c r="CS3" s="6">
+        <v>22</v>
+      </c>
+      <c r="CT3" s="6">
+        <v>22</v>
+      </c>
+      <c r="CU3" s="6">
+        <v>22</v>
+      </c>
+      <c r="CV3" s="6">
+        <v>22</v>
+      </c>
+      <c r="CW3" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="CZ3" s="3"/>
+      <c r="DC3" s="3"/>
+      <c r="DF3" s="3"/>
+      <c r="DI3" s="3"/>
+      <c r="DL3" s="3"/>
+      <c r="DO3" s="3"/>
+      <c r="DR3" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="DS3" s="3" t="s">
+        <v>297</v>
+      </c>
+      <c r="DT3" s="3" t="s">
+        <v>298</v>
+      </c>
+      <c r="DU3" s="3"/>
+      <c r="DX3" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="DY3" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="DZ3" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="EA3" s="3"/>
+      <c r="ED3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:134" x14ac:dyDescent="0.2">
+      <c r="A4" s="13" t="s">
+        <v>276</v>
+      </c>
+      <c r="B4" s="3"/>
+      <c r="E4" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="K4" s="3"/>
+      <c r="N4" s="3"/>
+      <c r="Q4" s="3"/>
+      <c r="T4" s="3"/>
+      <c r="W4" s="3"/>
+      <c r="Z4" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AC4" s="3"/>
+      <c r="AF4" s="3"/>
+      <c r="AI4" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="AK4" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL4" s="3"/>
+      <c r="AO4" s="3"/>
+      <c r="AR4" s="3"/>
+      <c r="AU4" s="3"/>
+      <c r="AX4" s="3"/>
+      <c r="BA4" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="BB4" t="s">
+        <v>283</v>
+      </c>
+      <c r="BC4" t="s">
+        <v>284</v>
+      </c>
+      <c r="BD4" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="BE4" s="3"/>
+      <c r="BF4" s="3"/>
+      <c r="BG4" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="BJ4" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="BM4" s="3"/>
+      <c r="BP4" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="BS4" s="4">
+        <v>425</v>
+      </c>
+      <c r="BT4" s="4">
+        <v>425</v>
+      </c>
+      <c r="BU4" s="4">
+        <v>425</v>
+      </c>
+      <c r="BV4" s="4">
+        <v>425</v>
+      </c>
+      <c r="BW4" s="4">
+        <v>425</v>
+      </c>
+      <c r="BX4" s="4">
+        <v>425</v>
+      </c>
+      <c r="BY4" s="5">
+        <v>37</v>
+      </c>
+      <c r="CE4" s="5">
+        <v>37</v>
+      </c>
+      <c r="CF4" s="5">
+        <v>37</v>
+      </c>
+      <c r="CG4" s="5">
+        <v>37</v>
+      </c>
+      <c r="CH4" s="5">
+        <v>37</v>
+      </c>
+      <c r="CI4" s="5">
+        <v>37</v>
+      </c>
+      <c r="CJ4" s="5">
+        <v>37</v>
+      </c>
+      <c r="CK4" s="6">
+        <v>30</v>
+      </c>
+      <c r="CQ4" s="6">
+        <v>22</v>
+      </c>
+      <c r="CR4" s="6">
+        <v>22</v>
+      </c>
+      <c r="CS4" s="6">
+        <v>22</v>
+      </c>
+      <c r="CT4" s="6">
+        <v>22</v>
+      </c>
+      <c r="CU4" s="6">
+        <v>22</v>
+      </c>
+      <c r="CV4" s="6">
+        <v>22</v>
+      </c>
+      <c r="CW4" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="CZ4" s="3"/>
+      <c r="DC4" s="3"/>
+      <c r="DF4" s="3"/>
+      <c r="DI4" s="3"/>
+      <c r="DL4" s="3"/>
+      <c r="DO4" s="3"/>
+      <c r="DR4" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="DU4" s="3"/>
+      <c r="DX4" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="EA4" s="3"/>
+      <c r="ED4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="5" spans="1:134" x14ac:dyDescent="0.2">
+      <c r="A5" s="12" t="s">
+        <v>277</v>
+      </c>
+      <c r="B5" s="3"/>
+      <c r="E5" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="K5" s="3"/>
+      <c r="N5" s="3"/>
+      <c r="Q5" s="3"/>
+      <c r="T5" s="3"/>
+      <c r="W5" s="3"/>
+      <c r="Z5" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AC5" s="3"/>
+      <c r="AF5" s="3"/>
+      <c r="AI5" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL5" s="3"/>
+      <c r="AO5" s="3"/>
+      <c r="AR5" s="3"/>
+      <c r="AU5" s="3"/>
+      <c r="AX5" s="3"/>
+      <c r="BA5" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="BB5" t="s">
+        <v>283</v>
+      </c>
+      <c r="BC5" t="s">
+        <v>284</v>
+      </c>
+      <c r="BD5" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="BE5" s="3"/>
+      <c r="BF5" s="3"/>
+      <c r="BG5" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="BJ5" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="BM5" s="3"/>
+      <c r="BP5" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="BS5" s="4">
+        <v>425</v>
+      </c>
+      <c r="BY5" s="5">
+        <v>37</v>
+      </c>
+      <c r="CE5" s="5">
+        <v>37</v>
+      </c>
+      <c r="CK5" s="6">
+        <v>30</v>
+      </c>
+      <c r="CQ5" s="6">
+        <v>22</v>
+      </c>
+      <c r="CW5" s="3" t="s">
+        <v>273</v>
+      </c>
+      <c r="CZ5" s="3"/>
+      <c r="DC5" s="3"/>
+      <c r="DF5" s="3"/>
+      <c r="DI5" s="3"/>
+      <c r="DL5" s="3"/>
+      <c r="DO5" s="3"/>
+      <c r="DR5" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="DU5" s="3"/>
+      <c r="DX5" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="EA5" s="3"/>
+      <c r="ED5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="6" spans="1:134" x14ac:dyDescent="0.2">
+      <c r="A6" s="13" t="s">
+        <v>278</v>
+      </c>
+      <c r="B6" s="3"/>
+      <c r="E6" s="3" t="s">
+        <v>262</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="K6" s="3"/>
+      <c r="N6" s="3"/>
+      <c r="Q6" s="3"/>
+      <c r="T6" s="3"/>
+      <c r="W6" s="3"/>
+      <c r="Z6" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AC6" s="3"/>
+      <c r="AF6" s="3"/>
+      <c r="AI6" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL6" s="3"/>
+      <c r="AO6" s="3"/>
+      <c r="AR6" s="3"/>
+      <c r="AU6" s="3"/>
+      <c r="AX6" s="3"/>
+      <c r="BA6" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="BB6" t="s">
+        <v>283</v>
+      </c>
+      <c r="BC6" t="s">
+        <v>284</v>
+      </c>
+      <c r="BD6" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="BE6" s="3"/>
+      <c r="BF6" s="3"/>
+      <c r="BG6" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="BJ6" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="BM6" s="3"/>
+      <c r="BP6" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="BS6" s="4">
+        <v>425</v>
+      </c>
+      <c r="BY6" s="5">
+        <v>37</v>
+      </c>
+      <c r="CE6" s="5">
+        <v>37</v>
+      </c>
+      <c r="CK6" s="6">
+        <v>30</v>
+      </c>
+      <c r="CQ6" s="6">
+        <v>22</v>
+      </c>
+      <c r="CW6" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="CZ6" s="3"/>
+      <c r="DC6" s="3"/>
+      <c r="DF6" s="3"/>
+      <c r="DI6" s="3"/>
+      <c r="DL6" s="3"/>
+      <c r="DO6" s="3"/>
+      <c r="DR6" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="DU6" s="3"/>
+      <c r="DX6" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="EA6" s="3"/>
+      <c r="ED6" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="7" spans="1:134" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>279</v>
+      </c>
+      <c r="B7" s="3"/>
+      <c r="E7" s="3" t="s">
+        <v>263</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="K7" s="3"/>
+      <c r="N7" s="3"/>
+      <c r="Q7" s="3"/>
+      <c r="T7" s="3"/>
+      <c r="W7" s="3"/>
+      <c r="Z7" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AC7" s="3"/>
+      <c r="AF7" s="3"/>
+      <c r="AI7" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL7" s="3"/>
+      <c r="AO7" s="3"/>
+      <c r="AR7" s="3"/>
+      <c r="AU7" s="3"/>
+      <c r="AX7" s="3"/>
+      <c r="BA7" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="BB7" t="s">
+        <v>283</v>
+      </c>
+      <c r="BC7" t="s">
+        <v>284</v>
+      </c>
+      <c r="BD7" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="BE7" s="3"/>
+      <c r="BF7" s="3"/>
+      <c r="BG7" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="BJ7" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="BM7" s="3"/>
+      <c r="BP7" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="BS7" s="4">
+        <v>425</v>
+      </c>
+      <c r="BY7" s="5">
+        <v>37</v>
+      </c>
+      <c r="CE7" s="5">
+        <v>37</v>
+      </c>
+      <c r="CK7" s="6">
+        <v>30</v>
+      </c>
+      <c r="CQ7" s="6">
+        <v>22</v>
+      </c>
+      <c r="CW7" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="CZ7" s="3"/>
+      <c r="DC7" s="3"/>
+      <c r="DF7" s="3"/>
+      <c r="DI7" s="3"/>
+      <c r="DL7" s="3"/>
+      <c r="DO7" s="3"/>
+      <c r="DR7" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="DU7" s="3"/>
+      <c r="DX7" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="EA7" s="3"/>
+      <c r="ED7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="8" spans="1:134" x14ac:dyDescent="0.2">
+      <c r="A8" s="13" t="s">
+        <v>280</v>
+      </c>
+      <c r="B8" s="3"/>
+      <c r="E8" s="3" t="s">
+        <v>264</v>
+      </c>
+      <c r="H8" s="3" t="s">
+        <v>265</v>
+      </c>
+      <c r="K8" s="3"/>
+      <c r="N8" s="3"/>
+      <c r="Q8" s="3"/>
+      <c r="T8" s="3"/>
+      <c r="W8" s="3"/>
+      <c r="Z8" s="3" t="s">
+        <v>272</v>
+      </c>
+      <c r="AC8" s="3"/>
+      <c r="AF8" s="3"/>
+      <c r="AI8" s="3" t="s">
+        <v>281</v>
+      </c>
+      <c r="AL8" s="3"/>
+      <c r="AO8" s="3"/>
+      <c r="AR8" s="3"/>
+      <c r="AU8" s="3"/>
+      <c r="AX8" s="3"/>
+      <c r="BA8" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="BB8" t="s">
+        <v>283</v>
+      </c>
+      <c r="BC8" t="s">
+        <v>284</v>
+      </c>
+      <c r="BD8" s="3" t="s">
+        <v>286</v>
+      </c>
+      <c r="BE8" s="3"/>
+      <c r="BF8" s="3"/>
+      <c r="BG8" s="3" t="s">
+        <v>287</v>
+      </c>
+      <c r="BJ8" s="3" t="s">
+        <v>293</v>
+      </c>
+      <c r="BM8" s="3"/>
+      <c r="BP8" s="3" t="s">
+        <v>294</v>
+      </c>
+      <c r="BS8" s="4">
+        <v>425</v>
+      </c>
+      <c r="BY8" s="5">
+        <v>37</v>
+      </c>
+      <c r="CE8" s="5">
+        <v>37</v>
+      </c>
+      <c r="CK8" s="6">
+        <v>30</v>
+      </c>
+      <c r="CQ8" s="6">
+        <v>22</v>
+      </c>
+      <c r="CW8" s="3" t="s">
+        <v>274</v>
+      </c>
+      <c r="CZ8" s="3"/>
+      <c r="DC8" s="3"/>
+      <c r="DF8" s="3"/>
+      <c r="DI8" s="3"/>
+      <c r="DL8" s="3"/>
+      <c r="DO8" s="3"/>
+      <c r="DR8" s="3" t="s">
+        <v>296</v>
+      </c>
+      <c r="DU8" s="3"/>
+      <c r="DX8" s="3" t="s">
+        <v>295</v>
+      </c>
+      <c r="EA8" s="3"/>
+      <c r="ED8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="B1:EC1"/>
+  </mergeCells>
+  <phoneticPr fontId="19" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA58125-CB37-0E46-A550-7C0D2A95EAFF}">
+  <dimension ref="A1:Z8"/>
+  <sheetViews>
+    <sheetView topLeftCell="N1" workbookViewId="0">
+      <selection activeCell="K16" sqref="K16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="51.1640625" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="57.33203125" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="29.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="58.1640625" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="64.33203125" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="37.33203125" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="48.1640625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="54.33203125" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="72.1640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="72.1640625" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="64.6640625" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="28.33203125" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="57.1640625" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="63.33203125" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="35.33203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="64" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="70.1640625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="37.33203125" hidden="1" customWidth="1"/>
+    <col min="21" max="21" width="48.1640625" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="54.33203125" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="50.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="58.33203125" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="64.5" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="15.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="10"/>
+      <c r="C1" s="10"/>
+      <c r="D1" s="10"/>
+      <c r="E1" s="10"/>
+      <c r="F1" s="10"/>
+      <c r="G1" s="10"/>
+      <c r="H1" s="10"/>
+      <c r="I1" s="10"/>
+      <c r="J1" s="10"/>
+      <c r="K1" s="10"/>
+      <c r="L1" s="10"/>
+      <c r="M1" s="10"/>
+      <c r="N1" s="10"/>
+      <c r="O1" s="10"/>
+      <c r="P1" s="10"/>
+      <c r="Q1" s="10"/>
+      <c r="R1" s="10"/>
+      <c r="S1" s="10"/>
+      <c r="T1" s="10"/>
+      <c r="U1" s="10"/>
+      <c r="V1" s="10"/>
+      <c r="W1" s="10"/>
+      <c r="X1" s="10"/>
+      <c r="Y1" s="10"/>
+      <c r="Z1" s="2"/>
+    </row>
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B2" t="s">
+        <v>173</v>
+      </c>
+      <c r="C2" t="s">
+        <v>174</v>
+      </c>
+      <c r="D2" t="s">
+        <v>175</v>
+      </c>
+      <c r="E2" t="s">
+        <v>167</v>
+      </c>
+      <c r="F2" t="s">
+        <v>168</v>
+      </c>
+      <c r="G2" t="s">
+        <v>169</v>
+      </c>
+      <c r="H2" t="s">
+        <v>170</v>
+      </c>
+      <c r="I2" t="s">
+        <v>171</v>
+      </c>
+      <c r="J2" t="s">
+        <v>172</v>
+      </c>
+      <c r="K2" t="s">
+        <v>164</v>
+      </c>
+      <c r="L2" t="s">
+        <v>165</v>
+      </c>
+      <c r="M2" t="s">
+        <v>166</v>
+      </c>
+      <c r="N2" t="s">
+        <v>161</v>
+      </c>
+      <c r="O2" t="s">
+        <v>162</v>
+      </c>
+      <c r="P2" t="s">
+        <v>163</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>155</v>
+      </c>
+      <c r="R2" t="s">
+        <v>156</v>
+      </c>
+      <c r="S2" t="s">
+        <v>157</v>
+      </c>
+      <c r="T2" t="s">
+        <v>158</v>
+      </c>
+      <c r="U2" t="s">
+        <v>159</v>
+      </c>
+      <c r="V2" t="s">
+        <v>160</v>
+      </c>
+      <c r="W2" t="s">
+        <v>152</v>
+      </c>
+      <c r="X2" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E3" s="7">
+        <v>80</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="L3" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="O3" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="P3" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>300</v>
+      </c>
+      <c r="R3" s="8">
+        <v>300</v>
+      </c>
+      <c r="S3" s="8">
+        <v>300</v>
+      </c>
+      <c r="T3" s="8">
+        <v>300</v>
+      </c>
+      <c r="U3" s="8">
+        <v>300</v>
+      </c>
+      <c r="V3" s="8">
+        <v>300</v>
+      </c>
+      <c r="W3" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>266</v>
+      </c>
+    </row>
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>267</v>
+      </c>
+      <c r="B4" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E4" s="7">
+        <v>78</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="L4" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q4" s="8">
+        <v>300</v>
+      </c>
+      <c r="R4" s="8">
+        <v>300</v>
+      </c>
+      <c r="S4" s="8">
+        <v>300</v>
+      </c>
+      <c r="T4" s="8">
+        <v>300</v>
+      </c>
+      <c r="U4" s="8">
+        <v>300</v>
+      </c>
+      <c r="V4" s="8">
+        <v>300</v>
+      </c>
+      <c r="W4" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>267</v>
+      </c>
+    </row>
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
+        <v>268</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E5" s="7">
+        <v>93</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q5" s="8">
+        <v>300</v>
+      </c>
+      <c r="W5" s="3" t="s">
+        <v>308</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>268</v>
+      </c>
+    </row>
+    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>269</v>
+      </c>
+      <c r="B6" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E6" s="7">
+        <v>82</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q6" s="8">
+        <v>300</v>
+      </c>
+      <c r="W6" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>269</v>
+      </c>
+    </row>
+    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>270</v>
+      </c>
+      <c r="B7" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E7" s="7">
+        <v>96</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q7" s="8">
+        <v>300</v>
+      </c>
+      <c r="W7" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>271</v>
+      </c>
+      <c r="B8" s="3" t="s">
+        <v>304</v>
+      </c>
+      <c r="E8" s="7">
+        <v>78</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>305</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="Q8" s="8">
+        <v>300</v>
+      </c>
+      <c r="W8" s="3" t="s">
+        <v>306</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>271</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="19" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD7966C-CFAD-E44B-9C7A-249E213AC34B}">
+  <dimension ref="A1:AX8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="AC11" sqref="AC11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="27.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="56.33203125" hidden="1" customWidth="1"/>
+    <col min="4" max="4" width="62.5" hidden="1" customWidth="1"/>
+    <col min="5" max="5" width="28.1640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="57" hidden="1" customWidth="1"/>
+    <col min="7" max="7" width="63.1640625" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="38" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="44.1640625" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="26" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="36.83203125" hidden="1" customWidth="1"/>
+    <col min="13" max="13" width="43" hidden="1" customWidth="1"/>
+    <col min="14" max="14" width="33" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="61.83203125" hidden="1" customWidth="1"/>
+    <col min="16" max="16" width="68" hidden="1" customWidth="1"/>
+    <col min="17" max="17" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="68.5" hidden="1" customWidth="1"/>
+    <col min="19" max="19" width="74.6640625" hidden="1" customWidth="1"/>
+    <col min="20" max="20" width="29.33203125" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="58" hidden="1" customWidth="1"/>
+    <col min="22" max="22" width="64.1640625" hidden="1" customWidth="1"/>
+    <col min="23" max="23" width="31.33203125" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="60.1640625" hidden="1" customWidth="1"/>
+    <col min="25" max="25" width="66.33203125" hidden="1" customWidth="1"/>
+    <col min="26" max="26" width="38.33203125" hidden="1" customWidth="1"/>
+    <col min="27" max="27" width="49.1640625" hidden="1" customWidth="1"/>
+    <col min="28" max="28" width="55.5" hidden="1" customWidth="1"/>
+    <col min="29" max="29" width="53.5" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="82.33203125" hidden="1" customWidth="1"/>
+    <col min="31" max="31" width="88.5" hidden="1" customWidth="1"/>
+    <col min="32" max="32" width="32.6640625" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="61.5" hidden="1" customWidth="1"/>
+    <col min="34" max="34" width="67.6640625" hidden="1" customWidth="1"/>
+    <col min="35" max="35" width="39.6640625" bestFit="1" customWidth="1"/>
+    <col min="36" max="36" width="68.33203125" hidden="1" customWidth="1"/>
+    <col min="37" max="37" width="74.5" hidden="1" customWidth="1"/>
+    <col min="38" max="38" width="43" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="71.83203125" hidden="1" customWidth="1"/>
+    <col min="40" max="40" width="78" hidden="1" customWidth="1"/>
+    <col min="41" max="41" width="25.83203125" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="54.5" hidden="1" customWidth="1"/>
+    <col min="43" max="43" width="60.83203125" hidden="1" customWidth="1"/>
+    <col min="44" max="44" width="43.83203125" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="60.6640625" hidden="1" customWidth="1"/>
+    <col min="47" max="47" width="66.83203125" hidden="1" customWidth="1"/>
+    <col min="48" max="48" width="34.5" bestFit="1" customWidth="1"/>
+    <col min="49" max="49" width="63.1640625" hidden="1" customWidth="1"/>
+    <col min="50" max="50" width="69.33203125" hidden="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="A1" s="1"/>
+      <c r="B1" s="10"/>
       <c r="C1" s="10"/>
       <c r="D1" s="10"/>
       <c r="E1" s="10"/>
@@ -2467,1451 +4290,461 @@
       <c r="AV1" s="10"/>
       <c r="AW1" s="10"/>
       <c r="AX1" s="10"/>
-      <c r="AY1" s="10"/>
-      <c r="AZ1" s="10"/>
-      <c r="BA1" s="10"/>
-      <c r="BB1" s="10"/>
-      <c r="BC1" s="10"/>
-      <c r="BD1" s="10"/>
-      <c r="BE1" s="10"/>
-      <c r="BF1" s="10"/>
-      <c r="BG1" s="10"/>
-      <c r="BH1" s="10"/>
-      <c r="BI1" s="10"/>
-      <c r="BJ1" s="10"/>
-      <c r="BK1" s="10"/>
-      <c r="BL1" s="10"/>
-      <c r="BM1" s="10"/>
-      <c r="BN1" s="10"/>
-      <c r="BO1" s="10"/>
-      <c r="BP1" s="10"/>
-      <c r="BQ1" s="10"/>
-      <c r="BR1" s="10"/>
-      <c r="BS1" s="10"/>
-      <c r="BT1" s="10"/>
-      <c r="BU1" s="10"/>
-      <c r="BV1" s="10"/>
-      <c r="BW1" s="10"/>
-      <c r="BX1" s="10"/>
-      <c r="BY1" s="10"/>
-      <c r="BZ1" s="10"/>
-      <c r="CA1" s="10"/>
-      <c r="CB1" s="10"/>
-      <c r="CC1" s="10"/>
-      <c r="CD1" s="10"/>
-      <c r="CE1" s="10"/>
-      <c r="CF1" s="10"/>
-      <c r="CG1" s="10"/>
-      <c r="CH1" s="10"/>
-      <c r="CI1" s="10"/>
-      <c r="CJ1" s="10"/>
-      <c r="CK1" s="10"/>
-      <c r="CL1" s="10"/>
-      <c r="CM1" s="10"/>
-      <c r="CN1" s="10"/>
-      <c r="CO1" s="10"/>
-      <c r="CP1" s="10"/>
-      <c r="CQ1" s="10"/>
-      <c r="CR1" s="10"/>
-      <c r="CS1" s="10"/>
-      <c r="CT1" s="10"/>
-      <c r="CU1" s="10"/>
-      <c r="CV1" s="10"/>
-      <c r="CW1" s="10"/>
-      <c r="CX1" s="10"/>
-      <c r="CY1" s="10"/>
-      <c r="CZ1" s="10"/>
-      <c r="DA1" s="10"/>
-      <c r="DB1" s="10"/>
-      <c r="DC1" s="10"/>
-      <c r="DD1" s="10"/>
-      <c r="DE1" s="10"/>
-      <c r="DF1" s="10"/>
-      <c r="DG1" s="10"/>
-      <c r="DH1" s="10"/>
-      <c r="DI1" s="10"/>
-      <c r="DJ1" s="10"/>
-      <c r="DK1" s="10"/>
-      <c r="DL1" s="10"/>
-      <c r="DM1" s="10"/>
-      <c r="DN1" s="10"/>
-      <c r="DO1" s="10"/>
-      <c r="DP1" s="10"/>
-      <c r="DQ1" s="10"/>
-      <c r="DR1" s="10"/>
-      <c r="DS1" s="10"/>
-      <c r="DT1" s="10"/>
-      <c r="DU1" s="10"/>
-      <c r="DV1" s="10"/>
-      <c r="DW1" s="10"/>
-      <c r="DX1" s="2"/>
     </row>
-    <row r="2" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>148</v>
+        <v>222</v>
       </c>
       <c r="C2" t="s">
-        <v>149</v>
+        <v>223</v>
       </c>
       <c r="D2" t="s">
-        <v>150</v>
+        <v>224</v>
       </c>
       <c r="E2" t="s">
-        <v>145</v>
+        <v>219</v>
       </c>
       <c r="F2" t="s">
-        <v>146</v>
+        <v>220</v>
       </c>
       <c r="G2" t="s">
-        <v>147</v>
+        <v>221</v>
       </c>
       <c r="H2" t="s">
-        <v>142</v>
+        <v>216</v>
       </c>
       <c r="I2" t="s">
-        <v>143</v>
+        <v>217</v>
       </c>
       <c r="J2" t="s">
-        <v>144</v>
+        <v>218</v>
       </c>
       <c r="K2" t="s">
-        <v>139</v>
+        <v>213</v>
       </c>
       <c r="L2" t="s">
-        <v>140</v>
+        <v>214</v>
       </c>
       <c r="M2" t="s">
-        <v>141</v>
+        <v>215</v>
       </c>
       <c r="N2" t="s">
-        <v>136</v>
+        <v>210</v>
       </c>
       <c r="O2" t="s">
-        <v>137</v>
+        <v>211</v>
       </c>
       <c r="P2" t="s">
-        <v>138</v>
+        <v>212</v>
       </c>
       <c r="Q2" t="s">
-        <v>133</v>
+        <v>207</v>
       </c>
       <c r="R2" t="s">
-        <v>134</v>
+        <v>208</v>
       </c>
       <c r="S2" t="s">
-        <v>135</v>
+        <v>209</v>
       </c>
       <c r="T2" t="s">
-        <v>130</v>
+        <v>204</v>
       </c>
       <c r="U2" t="s">
-        <v>131</v>
+        <v>205</v>
       </c>
       <c r="V2" t="s">
-        <v>132</v>
+        <v>206</v>
       </c>
       <c r="W2" t="s">
-        <v>127</v>
+        <v>198</v>
       </c>
       <c r="X2" t="s">
-        <v>128</v>
+        <v>199</v>
       </c>
       <c r="Y2" t="s">
-        <v>129</v>
+        <v>200</v>
       </c>
       <c r="Z2" t="s">
-        <v>124</v>
+        <v>201</v>
       </c>
       <c r="AA2" t="s">
-        <v>125</v>
+        <v>202</v>
       </c>
       <c r="AB2" t="s">
-        <v>126</v>
+        <v>203</v>
       </c>
       <c r="AC2" t="s">
-        <v>121</v>
+        <v>195</v>
       </c>
       <c r="AD2" t="s">
-        <v>122</v>
+        <v>196</v>
       </c>
       <c r="AE2" t="s">
-        <v>123</v>
+        <v>197</v>
       </c>
       <c r="AF2" t="s">
-        <v>118</v>
+        <v>192</v>
       </c>
       <c r="AG2" t="s">
-        <v>119</v>
+        <v>193</v>
       </c>
       <c r="AH2" t="s">
-        <v>120</v>
+        <v>194</v>
       </c>
       <c r="AI2" t="s">
-        <v>115</v>
+        <v>189</v>
       </c>
       <c r="AJ2" t="s">
-        <v>116</v>
+        <v>190</v>
       </c>
       <c r="AK2" t="s">
-        <v>117</v>
+        <v>191</v>
       </c>
       <c r="AL2" t="s">
-        <v>112</v>
+        <v>186</v>
       </c>
       <c r="AM2" t="s">
-        <v>113</v>
+        <v>187</v>
       </c>
       <c r="AN2" t="s">
-        <v>114</v>
+        <v>188</v>
       </c>
       <c r="AO2" t="s">
-        <v>109</v>
+        <v>183</v>
       </c>
       <c r="AP2" t="s">
-        <v>110</v>
+        <v>184</v>
       </c>
       <c r="AQ2" t="s">
-        <v>111</v>
+        <v>185</v>
       </c>
       <c r="AR2" t="s">
-        <v>106</v>
+        <v>182</v>
       </c>
       <c r="AS2" t="s">
-        <v>107</v>
+        <v>179</v>
       </c>
       <c r="AT2" t="s">
-        <v>108</v>
+        <v>180</v>
       </c>
       <c r="AU2" t="s">
-        <v>103</v>
+        <v>181</v>
       </c>
       <c r="AV2" t="s">
-        <v>104</v>
+        <v>176</v>
       </c>
       <c r="AW2" t="s">
-        <v>105</v>
+        <v>177</v>
       </c>
       <c r="AX2" t="s">
-        <v>100</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>101</v>
-      </c>
-      <c r="AZ2" t="s">
-        <v>102</v>
-      </c>
-      <c r="BA2" t="s">
-        <v>97</v>
-      </c>
-      <c r="BB2" t="s">
-        <v>98</v>
-      </c>
-      <c r="BC2" t="s">
-        <v>99</v>
-      </c>
-      <c r="BD2" t="s">
-        <v>94</v>
-      </c>
-      <c r="BE2" t="s">
-        <v>95</v>
-      </c>
-      <c r="BF2" t="s">
-        <v>96</v>
-      </c>
-      <c r="BG2" t="s">
-        <v>91</v>
-      </c>
-      <c r="BH2" t="s">
-        <v>92</v>
-      </c>
-      <c r="BI2" t="s">
-        <v>93</v>
-      </c>
-      <c r="BJ2" t="s">
-        <v>88</v>
-      </c>
-      <c r="BK2" t="s">
-        <v>89</v>
-      </c>
-      <c r="BL2" t="s">
-        <v>90</v>
-      </c>
-      <c r="BM2" t="s">
-        <v>82</v>
-      </c>
-      <c r="BN2" t="s">
-        <v>83</v>
-      </c>
-      <c r="BO2" t="s">
-        <v>84</v>
-      </c>
-      <c r="BP2" t="s">
-        <v>85</v>
-      </c>
-      <c r="BQ2" t="s">
-        <v>86</v>
-      </c>
-      <c r="BR2" t="s">
-        <v>87</v>
-      </c>
-      <c r="BS2" t="s">
-        <v>76</v>
-      </c>
-      <c r="BT2" t="s">
-        <v>77</v>
-      </c>
-      <c r="BU2" t="s">
-        <v>78</v>
-      </c>
-      <c r="BV2" t="s">
-        <v>79</v>
-      </c>
-      <c r="BW2" t="s">
-        <v>80</v>
-      </c>
-      <c r="BX2" t="s">
-        <v>81</v>
-      </c>
-      <c r="BY2" t="s">
-        <v>70</v>
-      </c>
-      <c r="BZ2" t="s">
-        <v>71</v>
-      </c>
-      <c r="CA2" t="s">
-        <v>72</v>
-      </c>
-      <c r="CB2" t="s">
-        <v>73</v>
-      </c>
-      <c r="CC2" t="s">
-        <v>74</v>
-      </c>
-      <c r="CD2" t="s">
-        <v>75</v>
-      </c>
-      <c r="CE2" t="s">
-        <v>64</v>
-      </c>
-      <c r="CF2" t="s">
-        <v>65</v>
-      </c>
-      <c r="CG2" t="s">
-        <v>66</v>
-      </c>
-      <c r="CH2" t="s">
-        <v>67</v>
-      </c>
-      <c r="CI2" t="s">
-        <v>68</v>
-      </c>
-      <c r="CJ2" t="s">
-        <v>69</v>
-      </c>
-      <c r="CK2" t="s">
-        <v>58</v>
-      </c>
-      <c r="CL2" t="s">
-        <v>59</v>
-      </c>
-      <c r="CM2" t="s">
-        <v>60</v>
-      </c>
-      <c r="CN2" t="s">
-        <v>61</v>
-      </c>
-      <c r="CO2" t="s">
-        <v>62</v>
-      </c>
-      <c r="CP2" t="s">
-        <v>63</v>
-      </c>
-      <c r="CQ2" t="s">
-        <v>55</v>
-      </c>
-      <c r="CR2" t="s">
-        <v>56</v>
-      </c>
-      <c r="CS2" t="s">
-        <v>57</v>
-      </c>
-      <c r="CT2" t="s">
-        <v>52</v>
-      </c>
-      <c r="CU2" t="s">
-        <v>53</v>
-      </c>
-      <c r="CV2" t="s">
-        <v>54</v>
-      </c>
-      <c r="CW2" t="s">
-        <v>49</v>
-      </c>
-      <c r="CX2" t="s">
-        <v>50</v>
-      </c>
-      <c r="CY2" t="s">
-        <v>51</v>
-      </c>
-      <c r="CZ2" t="s">
-        <v>46</v>
-      </c>
-      <c r="DA2" t="s">
-        <v>47</v>
-      </c>
-      <c r="DB2" t="s">
-        <v>48</v>
-      </c>
-      <c r="DC2" t="s">
-        <v>43</v>
-      </c>
-      <c r="DD2" t="s">
-        <v>44</v>
-      </c>
-      <c r="DE2" t="s">
-        <v>45</v>
-      </c>
-      <c r="DF2" t="s">
-        <v>40</v>
-      </c>
-      <c r="DG2" t="s">
-        <v>41</v>
-      </c>
-      <c r="DH2" t="s">
-        <v>42</v>
-      </c>
-      <c r="DI2" t="s">
-        <v>37</v>
-      </c>
-      <c r="DJ2" t="s">
-        <v>38</v>
-      </c>
-      <c r="DK2" t="s">
-        <v>39</v>
-      </c>
-      <c r="DL2" t="s">
-        <v>34</v>
-      </c>
-      <c r="DM2" t="s">
-        <v>35</v>
-      </c>
-      <c r="DN2" t="s">
-        <v>36</v>
-      </c>
-      <c r="DO2" t="s">
-        <v>31</v>
-      </c>
-      <c r="DP2" t="s">
-        <v>32</v>
-      </c>
-      <c r="DQ2" t="s">
-        <v>33</v>
-      </c>
-      <c r="DR2" t="s">
-        <v>28</v>
-      </c>
-      <c r="DS2" t="s">
-        <v>29</v>
-      </c>
-      <c r="DT2" t="s">
-        <v>30</v>
-      </c>
-      <c r="DU2" t="s">
-        <v>25</v>
-      </c>
-      <c r="DV2" t="s">
-        <v>26</v>
-      </c>
-      <c r="DW2" t="s">
-        <v>27</v>
-      </c>
-      <c r="DX2" t="s">
-        <v>24</v>
+        <v>178</v>
       </c>
     </row>
-    <row r="3" spans="1:128" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:50" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
+        <v>266</v>
+      </c>
+      <c r="B3" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="K3" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="N3" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="Q3" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="R3" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="T3" s="3" t="s">
+        <v>302</v>
+      </c>
+      <c r="W3" s="9"/>
+      <c r="AC3" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="AF3" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="AI3" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="AJ3" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="AL3" s="3"/>
+      <c r="AO3" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="AR3" s="3" t="s">
+        <v>256</v>
+      </c>
+      <c r="AS3" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="AV3" s="3"/>
+    </row>
+    <row r="4" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
         <v>267</v>
       </c>
-      <c r="B3" s="3"/>
-      <c r="E3" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="K3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="W3" s="3"/>
-      <c r="Z3" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="AC3" s="3"/>
-      <c r="AF3" s="3"/>
-      <c r="AI3" s="3"/>
-      <c r="AL3" s="3"/>
-      <c r="AO3" s="3"/>
-      <c r="AR3" s="3"/>
-      <c r="AU3" s="3"/>
-      <c r="AX3" s="3"/>
-      <c r="BA3" s="3"/>
-      <c r="BD3" s="3"/>
-      <c r="BG3" s="3"/>
-      <c r="BJ3" s="3"/>
-      <c r="BM3" s="4"/>
-      <c r="BS3" s="5"/>
-      <c r="BY3" s="5"/>
-      <c r="CE3" s="6"/>
-      <c r="CK3" s="6"/>
-      <c r="CQ3" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="CT3" s="3"/>
-      <c r="CW3" s="3"/>
-      <c r="CZ3" s="3"/>
-      <c r="DC3" s="3"/>
-      <c r="DF3" s="3"/>
-      <c r="DI3" s="3"/>
-      <c r="DL3" s="3"/>
-      <c r="DO3" s="3"/>
-      <c r="DR3" s="3"/>
-      <c r="DU3" s="3"/>
-      <c r="DX3" t="s">
-        <v>267</v>
-      </c>
+      <c r="B4" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="H4" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="K4" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="N4" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="Q4" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="R4" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="T4" s="3" t="s">
+        <v>303</v>
+      </c>
+      <c r="W4" s="9"/>
+      <c r="AC4" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="AF4" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="AI4" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="AJ4" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="AL4" s="3"/>
+      <c r="AO4" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="AR4" s="3" t="s">
+        <v>257</v>
+      </c>
+      <c r="AS4" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="AV4" s="3"/>
     </row>
-    <row r="4" spans="1:128" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+    <row r="5" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>268</v>
       </c>
-      <c r="B4" s="3"/>
-      <c r="E4" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="H4" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="K4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="W4" s="3"/>
-      <c r="Z4" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="AC4" s="3"/>
-      <c r="AF4" s="3"/>
-      <c r="AI4" s="3"/>
-      <c r="AL4" s="3"/>
-      <c r="AO4" s="3"/>
-      <c r="AR4" s="3"/>
-      <c r="AU4" s="3"/>
-      <c r="AX4" s="3"/>
-      <c r="BA4" s="3"/>
-      <c r="BD4" s="3"/>
-      <c r="BG4" s="3"/>
-      <c r="BJ4" s="3"/>
-      <c r="BM4" s="4"/>
-      <c r="BS4" s="5"/>
-      <c r="BY4" s="5"/>
-      <c r="CE4" s="6"/>
-      <c r="CK4" s="6"/>
-      <c r="CQ4" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="CT4" s="3"/>
-      <c r="CW4" s="3"/>
-      <c r="CZ4" s="3"/>
-      <c r="DC4" s="3"/>
-      <c r="DF4" s="3"/>
-      <c r="DI4" s="3"/>
-      <c r="DL4" s="3"/>
-      <c r="DO4" s="3"/>
-      <c r="DR4" s="3"/>
-      <c r="DU4" s="3"/>
-      <c r="DX4" t="s">
-        <v>268</v>
-      </c>
+      <c r="B5" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="H5" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="K5" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="N5" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="Q5" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="T5" s="3" t="s">
+        <v>299</v>
+      </c>
+      <c r="W5" s="9"/>
+      <c r="AC5" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="AF5" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="AI5" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="AL5" s="3"/>
+      <c r="AO5" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="AR5" s="3" t="s">
+        <v>258</v>
+      </c>
+      <c r="AS5" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="AV5" s="3"/>
     </row>
-    <row r="5" spans="1:128" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
+    <row r="6" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
         <v>269</v>
       </c>
-      <c r="B5" s="3"/>
-      <c r="E5" s="3" t="s">
-        <v>265</v>
-      </c>
-      <c r="H5" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="K5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="W5" s="3"/>
-      <c r="Z5" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="AC5" s="3"/>
-      <c r="AF5" s="3"/>
-      <c r="AI5" s="3"/>
-      <c r="AL5" s="3"/>
-      <c r="AO5" s="3"/>
-      <c r="AR5" s="3"/>
-      <c r="AU5" s="3"/>
-      <c r="AX5" s="3"/>
-      <c r="BA5" s="3"/>
-      <c r="BD5" s="3"/>
-      <c r="BG5" s="3"/>
-      <c r="BJ5" s="3"/>
-      <c r="BM5" s="4"/>
-      <c r="BS5" s="5"/>
-      <c r="BY5" s="5"/>
-      <c r="CE5" s="6"/>
-      <c r="CK5" s="6"/>
-      <c r="CQ5" s="3" t="s">
-        <v>274</v>
-      </c>
-      <c r="CT5" s="3"/>
-      <c r="CW5" s="3"/>
-      <c r="CZ5" s="3"/>
-      <c r="DC5" s="3"/>
-      <c r="DF5" s="3"/>
-      <c r="DI5" s="3"/>
-      <c r="DL5" s="3"/>
-      <c r="DO5" s="3"/>
-      <c r="DR5" s="3"/>
-      <c r="DU5" s="3"/>
-      <c r="DX5" t="s">
-        <v>269</v>
-      </c>
+      <c r="B6" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E6" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="H6" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="K6" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="N6" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="Q6" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="T6" s="3" t="s">
+        <v>300</v>
+      </c>
+      <c r="W6" s="9"/>
+      <c r="AC6" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="AF6" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="AI6" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="AL6" s="3"/>
+      <c r="AO6" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="AR6" s="3" t="s">
+        <v>259</v>
+      </c>
+      <c r="AS6" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="AV6" s="3"/>
     </row>
-    <row r="6" spans="1:128" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
+    <row r="7" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
         <v>270</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="E6" s="3" t="s">
-        <v>263</v>
-      </c>
-      <c r="H6" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="K6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="W6" s="3"/>
-      <c r="Z6" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="AC6" s="3"/>
-      <c r="AF6" s="3"/>
-      <c r="AI6" s="3"/>
-      <c r="AL6" s="3"/>
-      <c r="AO6" s="3"/>
-      <c r="AR6" s="3"/>
-      <c r="AU6" s="3"/>
-      <c r="AX6" s="3"/>
-      <c r="BA6" s="3"/>
-      <c r="BD6" s="3"/>
-      <c r="BG6" s="3"/>
-      <c r="BJ6" s="3"/>
-      <c r="BM6" s="4"/>
-      <c r="BS6" s="5"/>
-      <c r="BY6" s="5"/>
-      <c r="CE6" s="6"/>
-      <c r="CK6" s="6"/>
-      <c r="CQ6" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="CT6" s="3"/>
-      <c r="CW6" s="3"/>
-      <c r="CZ6" s="3"/>
-      <c r="DC6" s="3"/>
-      <c r="DF6" s="3"/>
-      <c r="DI6" s="3"/>
-      <c r="DL6" s="3"/>
-      <c r="DO6" s="3"/>
-      <c r="DR6" s="3"/>
-      <c r="DU6" s="3"/>
-      <c r="DX6" t="s">
-        <v>270</v>
-      </c>
+      <c r="B7" s="3" t="s">
+        <v>317</v>
+      </c>
+      <c r="E7" s="3" t="s">
+        <v>318</v>
+      </c>
+      <c r="H7" s="3" t="s">
+        <v>316</v>
+      </c>
+      <c r="K7" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="N7" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="Q7" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="T7" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="W7" s="9"/>
+      <c r="AC7" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="AF7" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="AI7" s="3" t="s">
+        <v>320</v>
+      </c>
+      <c r="AL7" s="3"/>
+      <c r="AO7" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="AR7" s="3" t="s">
+        <v>260</v>
+      </c>
+      <c r="AS7" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="AV7" s="3"/>
     </row>
-    <row r="7" spans="1:128" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
+    <row r="8" spans="1:50" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
         <v>271</v>
       </c>
-      <c r="B7" s="3"/>
-      <c r="E7" s="3" t="s">
-        <v>264</v>
-      </c>
-      <c r="H7" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="K7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="W7" s="3"/>
-      <c r="Z7" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="AC7" s="3"/>
-      <c r="AF7" s="3"/>
-      <c r="AI7" s="3"/>
-      <c r="AL7" s="3"/>
-      <c r="AO7" s="3"/>
-      <c r="AR7" s="3"/>
-      <c r="AU7" s="3"/>
-      <c r="AX7" s="3"/>
-      <c r="BA7" s="3"/>
-      <c r="BD7" s="3"/>
-      <c r="BG7" s="3"/>
-      <c r="BJ7" s="3"/>
-      <c r="BM7" s="4"/>
-      <c r="BS7" s="5"/>
-      <c r="BY7" s="5"/>
-      <c r="CE7" s="6"/>
-      <c r="CK7" s="6"/>
-      <c r="CQ7" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="CT7" s="3"/>
-      <c r="CW7" s="3"/>
-      <c r="CZ7" s="3"/>
-      <c r="DC7" s="3"/>
-      <c r="DF7" s="3"/>
-      <c r="DI7" s="3"/>
-      <c r="DL7" s="3"/>
-      <c r="DO7" s="3"/>
-      <c r="DR7" s="3"/>
-      <c r="DU7" s="3"/>
-      <c r="DX7" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="8" spans="1:128" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>272</v>
-      </c>
-      <c r="B8" s="3"/>
+      <c r="B8" s="3" t="s">
+        <v>317</v>
+      </c>
       <c r="E8" s="3" t="s">
-        <v>265</v>
+        <v>318</v>
       </c>
       <c r="H8" s="3" t="s">
-        <v>266</v>
-      </c>
-      <c r="K8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="W8" s="3"/>
-      <c r="Z8" s="3" t="s">
-        <v>273</v>
-      </c>
-      <c r="AC8" s="3"/>
-      <c r="AF8" s="3"/>
-      <c r="AI8" s="3"/>
+        <v>316</v>
+      </c>
+      <c r="K8" s="3" t="s">
+        <v>315</v>
+      </c>
+      <c r="N8" s="3" t="s">
+        <v>313</v>
+      </c>
+      <c r="Q8" s="3" t="s">
+        <v>314</v>
+      </c>
+      <c r="T8" s="3" t="s">
+        <v>301</v>
+      </c>
+      <c r="W8" s="9"/>
+      <c r="AC8" s="3" t="s">
+        <v>321</v>
+      </c>
+      <c r="AF8" s="3" t="s">
+        <v>319</v>
+      </c>
+      <c r="AI8" s="3" t="s">
+        <v>320</v>
+      </c>
       <c r="AL8" s="3"/>
-      <c r="AO8" s="3"/>
-      <c r="AR8" s="3"/>
-      <c r="AU8" s="3"/>
-      <c r="AX8" s="3"/>
-      <c r="BA8" s="3"/>
-      <c r="BD8" s="3"/>
-      <c r="BG8" s="3"/>
-      <c r="BJ8" s="3"/>
-      <c r="BM8" s="4"/>
-      <c r="BS8" s="5"/>
-      <c r="BY8" s="5"/>
-      <c r="CE8" s="6"/>
-      <c r="CK8" s="6"/>
-      <c r="CQ8" s="3" t="s">
-        <v>275</v>
-      </c>
-      <c r="CT8" s="3"/>
-      <c r="CW8" s="3"/>
-      <c r="CZ8" s="3"/>
-      <c r="DC8" s="3"/>
-      <c r="DF8" s="3"/>
-      <c r="DI8" s="3"/>
-      <c r="DL8" s="3"/>
-      <c r="DO8" s="3"/>
-      <c r="DR8" s="3"/>
-      <c r="DU8" s="3"/>
-      <c r="DX8" t="s">
-        <v>272</v>
-      </c>
+      <c r="AO8" s="3" t="s">
+        <v>312</v>
+      </c>
+      <c r="AR8" s="3" t="s">
+        <v>261</v>
+      </c>
+      <c r="AS8" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="AV8" s="3"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:DW1"/>
-  </mergeCells>
   <phoneticPr fontId="19" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EBA58125-CB37-0E46-A550-7C0D2A95EAFF}">
-  <dimension ref="A1:Z8"/>
-  <sheetViews>
-    <sheetView topLeftCell="Q1" workbookViewId="0">
-      <selection activeCell="Z3" sqref="Z3:Z8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.33203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="51.1640625" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="57.33203125" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="29.5" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="58.1640625" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="64.33203125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="37.33203125" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="48.1640625" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="54.33203125" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="29.83203125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="58.5" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="64.6640625" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="28.33203125" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="57.1640625" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="63.33203125" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="35.33203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="64" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="70.1640625" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="37.33203125" hidden="1" customWidth="1"/>
-    <col min="21" max="21" width="48.1640625" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="54.33203125" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="29.6640625" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="58.33203125" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="64.5" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="15.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="2"/>
-    </row>
-    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>173</v>
-      </c>
-      <c r="C2" t="s">
-        <v>174</v>
-      </c>
-      <c r="D2" t="s">
-        <v>175</v>
-      </c>
-      <c r="E2" t="s">
-        <v>167</v>
-      </c>
-      <c r="F2" t="s">
-        <v>168</v>
-      </c>
-      <c r="G2" t="s">
-        <v>169</v>
-      </c>
-      <c r="H2" t="s">
-        <v>170</v>
-      </c>
-      <c r="I2" t="s">
-        <v>171</v>
-      </c>
-      <c r="J2" t="s">
-        <v>172</v>
-      </c>
-      <c r="K2" t="s">
-        <v>164</v>
-      </c>
-      <c r="L2" t="s">
-        <v>165</v>
-      </c>
-      <c r="M2" t="s">
-        <v>166</v>
-      </c>
-      <c r="N2" t="s">
-        <v>161</v>
-      </c>
-      <c r="O2" t="s">
-        <v>162</v>
-      </c>
-      <c r="P2" t="s">
-        <v>163</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>155</v>
-      </c>
-      <c r="R2" t="s">
-        <v>156</v>
-      </c>
-      <c r="S2" t="s">
-        <v>157</v>
-      </c>
-      <c r="T2" t="s">
-        <v>158</v>
-      </c>
-      <c r="U2" t="s">
-        <v>159</v>
-      </c>
-      <c r="V2" t="s">
-        <v>160</v>
-      </c>
-      <c r="W2" t="s">
-        <v>152</v>
-      </c>
-      <c r="X2" t="s">
-        <v>153</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>154</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
-        <v>267</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="E3" s="7"/>
-      <c r="K3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="Q3" s="8"/>
-      <c r="W3" s="3"/>
-      <c r="Z3" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>268</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="E4" s="7"/>
-      <c r="K4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="Q4" s="8"/>
-      <c r="W4" s="3"/>
-      <c r="Z4" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>269</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="E5" s="7"/>
-      <c r="K5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="Q5" s="8"/>
-      <c r="W5" s="3"/>
-      <c r="Z5" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="6" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>270</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="E6" s="7"/>
-      <c r="K6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="Q6" s="8"/>
-      <c r="W6" s="3"/>
-      <c r="Z6" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="7" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>271</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="E7" s="7"/>
-      <c r="K7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="Q7" s="8"/>
-      <c r="W7" s="3"/>
-      <c r="Z7" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="8" spans="1:26" x14ac:dyDescent="0.2">
-      <c r="A8" t="s">
-        <v>272</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="E8" s="7"/>
-      <c r="K8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="Q8" s="8"/>
-      <c r="W8" s="3"/>
-      <c r="Z8" t="s">
-        <v>272</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
-    <tablePart r:id="rId1"/>
-  </tableParts>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DCD7966C-CFAD-E44B-9C7A-249E213AC34B}">
-  <dimension ref="A1:AY9"/>
-  <sheetViews>
-    <sheetView topLeftCell="AO1" workbookViewId="0">
-      <selection activeCell="AY3" sqref="AY3:AY8"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="27.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="56.33203125" hidden="1" customWidth="1"/>
-    <col min="4" max="4" width="62.5" hidden="1" customWidth="1"/>
-    <col min="5" max="5" width="28.1640625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="57" hidden="1" customWidth="1"/>
-    <col min="7" max="7" width="63.1640625" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="38" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="44.1640625" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="16.5" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="36.83203125" hidden="1" customWidth="1"/>
-    <col min="13" max="13" width="43" hidden="1" customWidth="1"/>
-    <col min="14" max="14" width="33" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="61.83203125" hidden="1" customWidth="1"/>
-    <col min="16" max="16" width="68" hidden="1" customWidth="1"/>
-    <col min="17" max="17" width="39.83203125" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="68.5" hidden="1" customWidth="1"/>
-    <col min="19" max="19" width="74.6640625" hidden="1" customWidth="1"/>
-    <col min="20" max="20" width="29.33203125" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="58" hidden="1" customWidth="1"/>
-    <col min="22" max="22" width="64.1640625" hidden="1" customWidth="1"/>
-    <col min="23" max="23" width="31.33203125" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="60.1640625" hidden="1" customWidth="1"/>
-    <col min="25" max="25" width="66.33203125" hidden="1" customWidth="1"/>
-    <col min="26" max="26" width="38.33203125" hidden="1" customWidth="1"/>
-    <col min="27" max="27" width="49.1640625" hidden="1" customWidth="1"/>
-    <col min="28" max="28" width="55.5" hidden="1" customWidth="1"/>
-    <col min="29" max="29" width="53.5" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="82.33203125" hidden="1" customWidth="1"/>
-    <col min="31" max="31" width="88.5" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="32.6640625" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="61.5" hidden="1" customWidth="1"/>
-    <col min="34" max="34" width="67.6640625" hidden="1" customWidth="1"/>
-    <col min="35" max="35" width="39.6640625" bestFit="1" customWidth="1"/>
-    <col min="36" max="36" width="68.33203125" hidden="1" customWidth="1"/>
-    <col min="37" max="37" width="74.5" hidden="1" customWidth="1"/>
-    <col min="38" max="38" width="43" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="71.83203125" hidden="1" customWidth="1"/>
-    <col min="40" max="40" width="78" hidden="1" customWidth="1"/>
-    <col min="41" max="41" width="25.83203125" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="54.5" hidden="1" customWidth="1"/>
-    <col min="43" max="43" width="60.83203125" hidden="1" customWidth="1"/>
-    <col min="44" max="44" width="43.83203125" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="31.83203125" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="60.6640625" hidden="1" customWidth="1"/>
-    <col min="47" max="47" width="66.83203125" hidden="1" customWidth="1"/>
-    <col min="48" max="48" width="34.5" bestFit="1" customWidth="1"/>
-    <col min="49" max="49" width="63.1640625" hidden="1" customWidth="1"/>
-    <col min="50" max="50" width="69.33203125" hidden="1" customWidth="1"/>
-    <col min="51" max="51" width="15.33203125" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A1" s="1"/>
-      <c r="B1" s="10" t="s">
-        <v>225</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="10"/>
-      <c r="AG1" s="10"/>
-      <c r="AH1" s="10"/>
-      <c r="AI1" s="10"/>
-      <c r="AJ1" s="10"/>
-      <c r="AK1" s="10"/>
-      <c r="AL1" s="10"/>
-      <c r="AM1" s="10"/>
-      <c r="AN1" s="10"/>
-      <c r="AO1" s="10"/>
-      <c r="AP1" s="10"/>
-      <c r="AQ1" s="10"/>
-      <c r="AR1" s="10"/>
-      <c r="AS1" s="10"/>
-      <c r="AT1" s="10"/>
-      <c r="AU1" s="10"/>
-      <c r="AV1" s="10"/>
-      <c r="AW1" s="10"/>
-      <c r="AX1" s="10"/>
-      <c r="AY1" s="2"/>
-    </row>
-    <row r="2" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>222</v>
-      </c>
-      <c r="C2" t="s">
-        <v>223</v>
-      </c>
-      <c r="D2" t="s">
-        <v>224</v>
-      </c>
-      <c r="E2" t="s">
-        <v>219</v>
-      </c>
-      <c r="F2" t="s">
-        <v>220</v>
-      </c>
-      <c r="G2" t="s">
-        <v>221</v>
-      </c>
-      <c r="H2" t="s">
-        <v>216</v>
-      </c>
-      <c r="I2" t="s">
-        <v>217</v>
-      </c>
-      <c r="J2" t="s">
-        <v>218</v>
-      </c>
-      <c r="K2" t="s">
-        <v>213</v>
-      </c>
-      <c r="L2" t="s">
-        <v>214</v>
-      </c>
-      <c r="M2" t="s">
-        <v>215</v>
-      </c>
-      <c r="N2" t="s">
-        <v>210</v>
-      </c>
-      <c r="O2" t="s">
-        <v>211</v>
-      </c>
-      <c r="P2" t="s">
-        <v>212</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>207</v>
-      </c>
-      <c r="R2" t="s">
-        <v>208</v>
-      </c>
-      <c r="S2" t="s">
-        <v>209</v>
-      </c>
-      <c r="T2" t="s">
-        <v>204</v>
-      </c>
-      <c r="U2" t="s">
-        <v>205</v>
-      </c>
-      <c r="V2" t="s">
-        <v>206</v>
-      </c>
-      <c r="W2" t="s">
-        <v>198</v>
-      </c>
-      <c r="X2" t="s">
-        <v>199</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>200</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>201</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>202</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>203</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>195</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>196</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>197</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>192</v>
-      </c>
-      <c r="AG2" t="s">
-        <v>193</v>
-      </c>
-      <c r="AH2" t="s">
-        <v>194</v>
-      </c>
-      <c r="AI2" t="s">
-        <v>189</v>
-      </c>
-      <c r="AJ2" t="s">
-        <v>190</v>
-      </c>
-      <c r="AK2" t="s">
-        <v>191</v>
-      </c>
-      <c r="AL2" t="s">
-        <v>186</v>
-      </c>
-      <c r="AM2" t="s">
-        <v>187</v>
-      </c>
-      <c r="AN2" t="s">
-        <v>188</v>
-      </c>
-      <c r="AO2" t="s">
-        <v>183</v>
-      </c>
-      <c r="AP2" t="s">
-        <v>184</v>
-      </c>
-      <c r="AQ2" t="s">
-        <v>185</v>
-      </c>
-      <c r="AR2" t="s">
-        <v>182</v>
-      </c>
-      <c r="AS2" t="s">
-        <v>179</v>
-      </c>
-      <c r="AT2" t="s">
-        <v>180</v>
-      </c>
-      <c r="AU2" t="s">
-        <v>181</v>
-      </c>
-      <c r="AV2" t="s">
-        <v>176</v>
-      </c>
-      <c r="AW2" t="s">
-        <v>177</v>
-      </c>
-      <c r="AX2" t="s">
-        <v>178</v>
-      </c>
-      <c r="AY2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>267</v>
-      </c>
-      <c r="B3" s="3"/>
-      <c r="E3" s="3"/>
-      <c r="H3" s="3"/>
-      <c r="K3" s="3"/>
-      <c r="N3" s="3"/>
-      <c r="Q3" s="3"/>
-      <c r="T3" s="3"/>
-      <c r="W3" s="9"/>
-      <c r="AC3" s="3"/>
-      <c r="AF3" s="3"/>
-      <c r="AI3" s="3"/>
-      <c r="AL3" s="3"/>
-      <c r="AO3" s="3"/>
-      <c r="AR3" s="3" t="s">
-        <v>257</v>
-      </c>
-      <c r="AS3" s="3"/>
-      <c r="AV3" s="3"/>
-      <c r="AY3" s="3" t="s">
-        <v>267</v>
-      </c>
-    </row>
-    <row r="4" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A4" s="3" t="s">
-        <v>268</v>
-      </c>
-      <c r="B4" s="3"/>
-      <c r="E4" s="3"/>
-      <c r="H4" s="3"/>
-      <c r="K4" s="3"/>
-      <c r="N4" s="3"/>
-      <c r="Q4" s="3"/>
-      <c r="T4" s="3"/>
-      <c r="W4" s="9"/>
-      <c r="AC4" s="3"/>
-      <c r="AF4" s="3"/>
-      <c r="AI4" s="3"/>
-      <c r="AL4" s="3"/>
-      <c r="AO4" s="3"/>
-      <c r="AR4" s="3" t="s">
-        <v>258</v>
-      </c>
-      <c r="AS4" s="3"/>
-      <c r="AV4" s="3"/>
-      <c r="AY4" s="3" t="s">
-        <v>268</v>
-      </c>
-    </row>
-    <row r="5" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A5" s="3" t="s">
-        <v>269</v>
-      </c>
-      <c r="B5" s="3"/>
-      <c r="E5" s="3"/>
-      <c r="H5" s="3"/>
-      <c r="K5" s="3"/>
-      <c r="N5" s="3"/>
-      <c r="Q5" s="3"/>
-      <c r="T5" s="3"/>
-      <c r="W5" s="9"/>
-      <c r="AC5" s="3"/>
-      <c r="AF5" s="3"/>
-      <c r="AI5" s="3"/>
-      <c r="AL5" s="3"/>
-      <c r="AO5" s="3"/>
-      <c r="AR5" s="3" t="s">
-        <v>259</v>
-      </c>
-      <c r="AS5" s="3"/>
-      <c r="AV5" s="3"/>
-      <c r="AY5" s="3" t="s">
-        <v>269</v>
-      </c>
-    </row>
-    <row r="6" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A6" s="3" t="s">
-        <v>270</v>
-      </c>
-      <c r="B6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="H6" s="3"/>
-      <c r="K6" s="3"/>
-      <c r="N6" s="3"/>
-      <c r="Q6" s="3"/>
-      <c r="T6" s="3"/>
-      <c r="W6" s="9"/>
-      <c r="AC6" s="3"/>
-      <c r="AF6" s="3"/>
-      <c r="AI6" s="3"/>
-      <c r="AL6" s="3"/>
-      <c r="AO6" s="3"/>
-      <c r="AR6" s="3" t="s">
-        <v>260</v>
-      </c>
-      <c r="AS6" s="3"/>
-      <c r="AV6" s="3"/>
-      <c r="AY6" s="3" t="s">
-        <v>270</v>
-      </c>
-    </row>
-    <row r="7" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A7" s="3" t="s">
-        <v>271</v>
-      </c>
-      <c r="B7" s="3"/>
-      <c r="E7" s="3"/>
-      <c r="H7" s="3"/>
-      <c r="K7" s="3"/>
-      <c r="N7" s="3"/>
-      <c r="Q7" s="3"/>
-      <c r="T7" s="3"/>
-      <c r="W7" s="9"/>
-      <c r="AC7" s="3"/>
-      <c r="AF7" s="3"/>
-      <c r="AI7" s="3"/>
-      <c r="AL7" s="3"/>
-      <c r="AO7" s="3"/>
-      <c r="AR7" s="3" t="s">
-        <v>261</v>
-      </c>
-      <c r="AS7" s="3"/>
-      <c r="AV7" s="3"/>
-      <c r="AY7" s="3" t="s">
-        <v>271</v>
-      </c>
-    </row>
-    <row r="8" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A8" s="3" t="s">
-        <v>272</v>
-      </c>
-      <c r="B8" s="3"/>
-      <c r="E8" s="3"/>
-      <c r="H8" s="3"/>
-      <c r="K8" s="3"/>
-      <c r="N8" s="3"/>
-      <c r="Q8" s="3"/>
-      <c r="T8" s="3"/>
-      <c r="W8" s="9"/>
-      <c r="AC8" s="3"/>
-      <c r="AF8" s="3"/>
-      <c r="AI8" s="3"/>
-      <c r="AL8" s="3"/>
-      <c r="AO8" s="3"/>
-      <c r="AR8" s="3" t="s">
-        <v>262</v>
-      </c>
-      <c r="AS8" s="3"/>
-      <c r="AV8" s="3"/>
-      <c r="AY8" s="3" t="s">
-        <v>272</v>
-      </c>
-    </row>
-    <row r="9" spans="1:51" x14ac:dyDescent="0.2">
-      <c r="A9" s="3"/>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="B1:AX1"/>
-  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
     <tablePart r:id="rId1"/>
@@ -3921,15 +4754,15 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9B1A2CB9-5E18-B848-9C59-2CAC936918FE}">
-  <dimension ref="A1:AF8"/>
+  <dimension ref="A1:AG8"/>
   <sheetViews>
-    <sheetView topLeftCell="T1" workbookViewId="0">
-      <selection activeCell="W16" sqref="W16"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="43.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="33.5" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="62.33203125" hidden="1" customWidth="1"/>
     <col min="4" max="4" width="68.5" hidden="1" customWidth="1"/>
@@ -3960,250 +4793,251 @@
     <col min="29" max="29" width="39" bestFit="1" customWidth="1"/>
     <col min="30" max="30" width="67.83203125" hidden="1" customWidth="1"/>
     <col min="31" max="31" width="74" hidden="1" customWidth="1"/>
-    <col min="32" max="32" width="15.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
-      <c r="B1" s="10" t="s">
+      <c r="B1" s="11" t="s">
+        <v>255</v>
+      </c>
+      <c r="C1" s="11"/>
+      <c r="D1" s="11"/>
+      <c r="E1" s="11"/>
+      <c r="F1" s="11"/>
+      <c r="G1" s="11"/>
+      <c r="H1" s="11"/>
+      <c r="I1" s="11"/>
+      <c r="J1" s="11"/>
+      <c r="K1" s="11"/>
+      <c r="L1" s="11"/>
+      <c r="M1" s="11"/>
+      <c r="N1" s="11"/>
+      <c r="O1" s="11"/>
+      <c r="P1" s="11"/>
+      <c r="Q1" s="11"/>
+      <c r="R1" s="11"/>
+      <c r="S1" s="11"/>
+      <c r="T1" s="11"/>
+      <c r="U1" s="11"/>
+      <c r="V1" s="11"/>
+      <c r="W1" s="11"/>
+      <c r="X1" s="11"/>
+      <c r="Y1" s="11"/>
+      <c r="Z1" s="11"/>
+      <c r="AA1" s="11"/>
+      <c r="AB1" s="11"/>
+      <c r="AC1" s="11"/>
+      <c r="AD1" s="11"/>
+      <c r="AE1" s="11"/>
+    </row>
+    <row r="2" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>182</v>
+      </c>
+      <c r="B2" t="s">
+        <v>252</v>
+      </c>
+      <c r="C2" t="s">
+        <v>253</v>
+      </c>
+      <c r="D2" t="s">
+        <v>254</v>
+      </c>
+      <c r="E2" t="s">
+        <v>249</v>
+      </c>
+      <c r="F2" t="s">
+        <v>250</v>
+      </c>
+      <c r="G2" t="s">
+        <v>251</v>
+      </c>
+      <c r="H2" t="s">
+        <v>246</v>
+      </c>
+      <c r="I2" t="s">
+        <v>247</v>
+      </c>
+      <c r="J2" t="s">
+        <v>248</v>
+      </c>
+      <c r="K2" t="s">
+        <v>243</v>
+      </c>
+      <c r="L2" t="s">
+        <v>244</v>
+      </c>
+      <c r="M2" t="s">
+        <v>245</v>
+      </c>
+      <c r="N2" t="s">
+        <v>240</v>
+      </c>
+      <c r="O2" t="s">
+        <v>241</v>
+      </c>
+      <c r="P2" t="s">
+        <v>242</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>237</v>
+      </c>
+      <c r="R2" t="s">
+        <v>238</v>
+      </c>
+      <c r="S2" t="s">
+        <v>239</v>
+      </c>
+      <c r="T2" t="s">
+        <v>234</v>
+      </c>
+      <c r="U2" t="s">
+        <v>235</v>
+      </c>
+      <c r="V2" t="s">
+        <v>236</v>
+      </c>
+      <c r="W2" t="s">
+        <v>231</v>
+      </c>
+      <c r="X2" t="s">
+        <v>232</v>
+      </c>
+      <c r="Y2" t="s">
+        <v>233</v>
+      </c>
+      <c r="Z2" t="s">
+        <v>228</v>
+      </c>
+      <c r="AA2" t="s">
+        <v>229</v>
+      </c>
+      <c r="AB2" t="s">
+        <v>230</v>
+      </c>
+      <c r="AC2" t="s">
+        <v>225</v>
+      </c>
+      <c r="AD2" t="s">
+        <v>226</v>
+      </c>
+      <c r="AE2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="3" spans="1:31" x14ac:dyDescent="0.2">
+      <c r="A3" s="3" t="s">
         <v>256</v>
-      </c>
-      <c r="C1" s="10"/>
-      <c r="D1" s="10"/>
-      <c r="E1" s="10"/>
-      <c r="F1" s="10"/>
-      <c r="G1" s="10"/>
-      <c r="H1" s="10"/>
-      <c r="I1" s="10"/>
-      <c r="J1" s="10"/>
-      <c r="K1" s="10"/>
-      <c r="L1" s="10"/>
-      <c r="M1" s="10"/>
-      <c r="N1" s="10"/>
-      <c r="O1" s="10"/>
-      <c r="P1" s="10"/>
-      <c r="Q1" s="10"/>
-      <c r="R1" s="10"/>
-      <c r="S1" s="10"/>
-      <c r="T1" s="10"/>
-      <c r="U1" s="10"/>
-      <c r="V1" s="10"/>
-      <c r="W1" s="10"/>
-      <c r="X1" s="10"/>
-      <c r="Y1" s="10"/>
-      <c r="Z1" s="10"/>
-      <c r="AA1" s="10"/>
-      <c r="AB1" s="10"/>
-      <c r="AC1" s="10"/>
-      <c r="AD1" s="10"/>
-      <c r="AE1" s="10"/>
-      <c r="AF1" s="2"/>
-    </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>23</v>
-      </c>
-      <c r="B2" t="s">
-        <v>253</v>
-      </c>
-      <c r="C2" t="s">
-        <v>254</v>
-      </c>
-      <c r="D2" t="s">
-        <v>255</v>
-      </c>
-      <c r="E2" t="s">
-        <v>250</v>
-      </c>
-      <c r="F2" t="s">
-        <v>251</v>
-      </c>
-      <c r="G2" t="s">
-        <v>252</v>
-      </c>
-      <c r="H2" t="s">
-        <v>247</v>
-      </c>
-      <c r="I2" t="s">
-        <v>248</v>
-      </c>
-      <c r="J2" t="s">
-        <v>249</v>
-      </c>
-      <c r="K2" t="s">
-        <v>244</v>
-      </c>
-      <c r="L2" t="s">
-        <v>245</v>
-      </c>
-      <c r="M2" t="s">
-        <v>246</v>
-      </c>
-      <c r="N2" t="s">
-        <v>241</v>
-      </c>
-      <c r="O2" t="s">
-        <v>242</v>
-      </c>
-      <c r="P2" t="s">
-        <v>243</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>238</v>
-      </c>
-      <c r="R2" t="s">
-        <v>239</v>
-      </c>
-      <c r="S2" t="s">
-        <v>240</v>
-      </c>
-      <c r="T2" t="s">
-        <v>235</v>
-      </c>
-      <c r="U2" t="s">
-        <v>236</v>
-      </c>
-      <c r="V2" t="s">
-        <v>237</v>
-      </c>
-      <c r="W2" t="s">
-        <v>232</v>
-      </c>
-      <c r="X2" t="s">
-        <v>233</v>
-      </c>
-      <c r="Y2" t="s">
-        <v>234</v>
-      </c>
-      <c r="Z2" t="s">
-        <v>229</v>
-      </c>
-      <c r="AA2" t="s">
-        <v>230</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>231</v>
-      </c>
-      <c r="AC2" t="s">
-        <v>226</v>
-      </c>
-      <c r="AD2" t="s">
-        <v>227</v>
-      </c>
-      <c r="AE2" t="s">
-        <v>228</v>
-      </c>
-      <c r="AF2" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.2">
-      <c r="A3" s="3" t="s">
-        <v>267</v>
       </c>
       <c r="B3" s="3"/>
       <c r="E3" s="3"/>
       <c r="H3" s="3"/>
-      <c r="K3" s="3"/>
+      <c r="K3" s="3" t="s">
+        <v>322</v>
+      </c>
       <c r="N3" s="3"/>
       <c r="Q3" s="3"/>
-      <c r="T3" s="3"/>
+      <c r="T3" s="3" t="s">
+        <v>323</v>
+      </c>
       <c r="W3" s="3"/>
       <c r="Z3" s="3"/>
       <c r="AC3" s="3"/>
-      <c r="AF3" s="3" t="s">
-        <v>267</v>
-      </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A4" s="3" t="s">
-        <v>268</v>
+        <v>257</v>
       </c>
       <c r="B4" s="3"/>
       <c r="E4" s="3"/>
       <c r="H4" s="3"/>
-      <c r="K4" s="3"/>
+      <c r="K4" s="3" t="s">
+        <v>322</v>
+      </c>
       <c r="N4" s="3"/>
       <c r="Q4" s="3"/>
-      <c r="T4" s="3"/>
+      <c r="T4" s="3" t="s">
+        <v>323</v>
+      </c>
       <c r="W4" s="3"/>
       <c r="Z4" s="3"/>
       <c r="AC4" s="3"/>
-      <c r="AF4" s="3" t="s">
-        <v>268</v>
-      </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A5" s="3" t="s">
-        <v>269</v>
+        <v>258</v>
       </c>
       <c r="B5" s="3"/>
       <c r="E5" s="3"/>
       <c r="H5" s="3"/>
-      <c r="K5" s="3"/>
+      <c r="K5" s="3" t="s">
+        <v>322</v>
+      </c>
       <c r="N5" s="3"/>
       <c r="Q5" s="3"/>
-      <c r="T5" s="3"/>
+      <c r="T5" s="3" t="s">
+        <v>323</v>
+      </c>
       <c r="W5" s="3"/>
       <c r="Z5" s="3"/>
       <c r="AC5" s="3"/>
-      <c r="AF5" s="3" t="s">
-        <v>269</v>
-      </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A6" s="3" t="s">
-        <v>270</v>
+        <v>259</v>
       </c>
       <c r="B6" s="3"/>
       <c r="E6" s="3"/>
       <c r="H6" s="3"/>
-      <c r="K6" s="3"/>
+      <c r="K6" s="3" t="s">
+        <v>322</v>
+      </c>
       <c r="N6" s="3"/>
       <c r="Q6" s="3"/>
-      <c r="T6" s="3"/>
+      <c r="T6" s="3" t="s">
+        <v>323</v>
+      </c>
       <c r="W6" s="3"/>
       <c r="Z6" s="3"/>
       <c r="AC6" s="3"/>
-      <c r="AF6" s="3" t="s">
-        <v>270</v>
-      </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A7" s="3" t="s">
-        <v>271</v>
+        <v>260</v>
       </c>
       <c r="B7" s="3"/>
       <c r="E7" s="3"/>
       <c r="H7" s="3"/>
-      <c r="K7" s="3"/>
+      <c r="K7" s="3" t="s">
+        <v>322</v>
+      </c>
       <c r="N7" s="3"/>
       <c r="Q7" s="3"/>
-      <c r="T7" s="3"/>
+      <c r="T7" s="3" t="s">
+        <v>323</v>
+      </c>
       <c r="W7" s="3"/>
       <c r="Z7" s="3"/>
       <c r="AC7" s="3"/>
-      <c r="AF7" s="3" t="s">
-        <v>271</v>
-      </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:31" x14ac:dyDescent="0.2">
       <c r="A8" s="3" t="s">
-        <v>272</v>
+        <v>261</v>
       </c>
       <c r="B8" s="3"/>
       <c r="E8" s="3"/>
       <c r="H8" s="3"/>
-      <c r="K8" s="3"/>
+      <c r="K8" s="3" t="s">
+        <v>322</v>
+      </c>
       <c r="N8" s="3"/>
       <c r="Q8" s="3"/>
-      <c r="T8" s="3"/>
+      <c r="T8" s="3" t="s">
+        <v>323</v>
+      </c>
       <c r="W8" s="3"/>
       <c r="Z8" s="3"/>
       <c r="AC8" s="3"/>
-      <c r="AF8" s="3" t="s">
-        <v>272</v>
-      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>